<commit_message>
nuevas integraciones para Almacen y sus Recursos
</commit_message>
<xml_diff>
--- a/QuerysAñadidas.xlsx
+++ b/QuerysAñadidas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ncano\Desktop\inacons-frontend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{89F9BCBE-E6E0-4B3D-909F-B8363EE96316}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A924790-C2FD-4D30-9DFF-647C38BF6D47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="7905" windowWidth="28800" windowHeight="7800" xr2:uid="{C2939682-D91A-4BD3-AD71-BB0CA9127A74}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C2939682-D91A-4BD3-AD71-BB0CA9127A74}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -561,7 +561,7 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor theme="8" tint="0.59999389629810485"/>
+          <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
     </dxf>
@@ -577,7 +577,7 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor rgb="FFFFFF00"/>
+          <bgColor theme="8" tint="0.59999389629810485"/>
         </patternFill>
       </fill>
     </dxf>
@@ -638,11 +638,11 @@
   </sortState>
   <tableColumns count="6">
     <tableColumn id="2" xr3:uid="{9A32BBF7-304C-49E3-AE42-106F9CEEC961}" name="Listar" dataDxfId="5"/>
-    <tableColumn id="1" xr3:uid="{C011CDE6-69F6-4DE8-B5A1-2E6AF137E527}" name="Buscar por Id" dataDxfId="0"/>
-    <tableColumn id="3" xr3:uid="{7FF29903-9CE1-4BD7-849F-3471C53EC880}" name="Agregar" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{30FB0AF3-511C-4F53-947B-89013B98F552}" name="Actualizar" dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{C011CDE6-69F6-4DE8-B5A1-2E6AF137E527}" name="Buscar por Id" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{7FF29903-9CE1-4BD7-849F-3471C53EC880}" name="Agregar" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{30FB0AF3-511C-4F53-947B-89013B98F552}" name="Actualizar" dataDxfId="2"/>
     <tableColumn id="5" xr3:uid="{D1A0B2A0-09FE-47C4-9132-E8B248D6B643}" name="Borrar" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{C7C99C68-6028-4378-A991-EDE5C1106AD0}" name="Adiconal" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{C7C99C68-6028-4378-A991-EDE5C1106AD0}" name="Adiconal" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -967,8 +967,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DE2F4B0-FA8B-45A2-B9E1-1433688D7CE8}">
   <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1393,33 +1393,33 @@
       <c r="F24" s="4"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="4" t="s">
+      <c r="A25" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B25" s="4"/>
-      <c r="C25" s="4" t="s">
+      <c r="C25" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D25" s="4" t="s">
+      <c r="D25" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="E25" s="4" t="s">
+      <c r="E25" s="1" t="s">
         <v>84</v>
       </c>
       <c r="F25" s="4"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="4" t="s">
+      <c r="A26" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B26" s="4"/>
-      <c r="C26" s="4" t="s">
+      <c r="C26" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D26" s="4" t="s">
+      <c r="D26" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="E26" s="4" t="s">
+      <c r="E26" s="1" t="s">
         <v>85</v>
       </c>
       <c r="F26" s="4"/>
@@ -1441,33 +1441,33 @@
       <c r="F27" s="4"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="4" t="s">
+      <c r="A28" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B28" s="4"/>
-      <c r="C28" s="4" t="s">
+      <c r="C28" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="D28" s="4" t="s">
+      <c r="D28" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="E28" s="4" t="s">
+      <c r="E28" s="1" t="s">
         <v>93</v>
       </c>
       <c r="F28" s="4"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="4" t="s">
+      <c r="A29" s="1" t="s">
         <v>35</v>
       </c>
       <c r="B29" s="4"/>
-      <c r="C29" s="4" t="s">
+      <c r="C29" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="D29" s="4" t="s">
+      <c r="D29" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="E29" s="4" t="s">
+      <c r="E29" s="1" t="s">
         <v>95</v>
       </c>
       <c r="F29" s="4"/>

</xml_diff>

<commit_message>
APIS compras movimientos almacen centro de costos añadidos
</commit_message>
<xml_diff>
--- a/QuerysAñadidas.xlsx
+++ b/QuerysAñadidas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ncano\Desktop\inacons-frontend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CB28269-3E97-4A43-AF1A-8E443C33F469}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BB4E110-F79F-4ED6-AFAB-6D99AE66E964}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C2939682-D91A-4BD3-AD71-BB0CA9127A74}"/>
   </bookViews>
@@ -650,7 +650,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1356,11 +1356,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DE2F4B0-FA8B-45A2-B9E1-1433688D7CE8}">
   <dimension ref="A1:H123"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="E50" sqref="E50"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="50.625" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="54.375" style="2" bestFit="1" customWidth="1"/>
@@ -1375,7 +1375,7 @@
     <col min="11" max="16384" width="11" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>120</v>
       </c>
@@ -1395,7 +1395,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="6"/>
       <c r="B2" s="6" t="s">
         <v>92</v>
@@ -1405,7 +1405,7 @@
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
@@ -1425,7 +1425,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>14</v>
       </c>
@@ -1445,7 +1445,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>12</v>
       </c>
@@ -1465,7 +1465,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>16</v>
       </c>
@@ -1479,7 +1479,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>17</v>
       </c>
@@ -1499,7 +1499,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>23</v>
       </c>
@@ -1517,7 +1517,7 @@
       </c>
       <c r="F8" s="16"/>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>24</v>
       </c>
@@ -1535,7 +1535,7 @@
       </c>
       <c r="F9" s="16"/>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>27</v>
       </c>
@@ -1549,7 +1549,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>28</v>
       </c>
@@ -1566,7 +1566,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="12" spans="1:7" s="5" customFormat="1">
+    <row r="12" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="8" t="s">
         <v>29</v>
       </c>
@@ -1587,7 +1587,7 @@
       </c>
       <c r="G12" s="18"/>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="10" t="s">
         <v>31</v>
       </c>
@@ -1607,7 +1607,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="10" t="s">
         <v>31</v>
       </c>
@@ -1627,7 +1627,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="10" t="s">
         <v>31</v>
       </c>
@@ -1647,7 +1647,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="10" t="s">
         <v>31</v>
       </c>
@@ -1667,7 +1667,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>32</v>
       </c>
@@ -1684,7 +1684,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>33</v>
       </c>
@@ -1701,7 +1701,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>37</v>
       </c>
@@ -1715,7 +1715,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>38</v>
       </c>
@@ -1729,7 +1729,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>39</v>
       </c>
@@ -1743,7 +1743,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
         <v>22</v>
       </c>
@@ -1757,7 +1757,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>19</v>
       </c>
@@ -1775,7 +1775,7 @@
       </c>
       <c r="F23" s="16"/>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>20</v>
       </c>
@@ -1795,7 +1795,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>26</v>
       </c>
@@ -1811,7 +1811,7 @@
       </c>
       <c r="F25" s="16"/>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
         <v>25</v>
       </c>
@@ -1827,7 +1827,7 @@
       </c>
       <c r="F26" s="16"/>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>34</v>
       </c>
@@ -1843,7 +1843,7 @@
       </c>
       <c r="F27" s="16"/>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>35</v>
       </c>
@@ -1859,93 +1859,93 @@
       </c>
       <c r="F28" s="16"/>
     </row>
-    <row r="29" spans="1:6">
-      <c r="A29" s="7" t="s">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B29" s="7" t="s">
+      <c r="B29" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C29" s="7" t="s">
+      <c r="C29" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="D29" s="7" t="s">
+      <c r="D29" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="E29" s="7" t="s">
+      <c r="E29" s="3" t="s">
         <v>86</v>
       </c>
       <c r="F29" s="16"/>
     </row>
-    <row r="30" spans="1:6">
-      <c r="A30" s="7" t="s">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B30" s="7"/>
-      <c r="C30" s="7" t="s">
+      <c r="B30" s="16"/>
+      <c r="C30" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D30" s="7" t="s">
+      <c r="D30" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="E30" s="7" t="s">
+      <c r="E30" s="3" t="s">
         <v>82</v>
       </c>
       <c r="F30" s="16"/>
     </row>
-    <row r="31" spans="1:6">
-      <c r="A31" s="7" t="s">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A31" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="B31" s="7" t="s">
+      <c r="B31" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="C31" s="7" t="s">
+      <c r="C31" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="D31" s="7" t="s">
+      <c r="D31" s="3" t="s">
         <v>185</v>
       </c>
-      <c r="E31" s="7" t="s">
+      <c r="E31" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="F31" s="7" t="s">
+      <c r="F31" s="3" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="32" spans="1:6">
-      <c r="A32" s="7" t="s">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32" s="3" t="s">
         <v>136</v>
       </c>
       <c r="B32" s="16"/>
-      <c r="C32" s="7" t="s">
+      <c r="C32" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="D32" s="7" t="s">
+      <c r="D32" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="E32" s="7" t="s">
+      <c r="E32" s="3" t="s">
         <v>172</v>
       </c>
       <c r="F32" s="16"/>
     </row>
-    <row r="33" spans="1:6">
-      <c r="A33" s="7" t="s">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A33" s="3" t="s">
         <v>137</v>
       </c>
       <c r="B33" s="16"/>
-      <c r="C33" s="7" t="s">
+      <c r="C33" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="D33" s="7" t="s">
+      <c r="D33" s="3" t="s">
         <v>187</v>
       </c>
-      <c r="E33" s="7" t="s">
+      <c r="E33" s="3" t="s">
         <v>173</v>
       </c>
       <c r="F33" s="16"/>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
         <v>140</v>
       </c>
@@ -1961,9 +1961,9 @@
       <c r="E34" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="F34" s="3"/>
-    </row>
-    <row r="35" spans="1:6">
+      <c r="F34" s="16"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="7" t="s">
         <v>139</v>
       </c>
@@ -1983,7 +1983,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="36" spans="1:6">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
         <v>141</v>
       </c>
@@ -2001,23 +2001,23 @@
       </c>
       <c r="F36" s="16"/>
     </row>
-    <row r="37" spans="1:6">
-      <c r="A37" s="7" t="s">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A37" s="3" t="s">
         <v>143</v>
       </c>
       <c r="B37" s="16"/>
-      <c r="C37" s="7" t="s">
+      <c r="C37" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="D37" s="7" t="s">
+      <c r="D37" s="3" t="s">
         <v>192</v>
       </c>
-      <c r="E37" s="7" t="s">
+      <c r="E37" s="3" t="s">
         <v>177</v>
       </c>
       <c r="F37" s="16"/>
     </row>
-    <row r="38" spans="1:6">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
         <v>146</v>
       </c>
@@ -2035,7 +2035,7 @@
       </c>
       <c r="F38" s="16"/>
     </row>
-    <row r="39" spans="1:6">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
         <v>144</v>
       </c>
@@ -2050,25 +2050,25 @@
       </c>
       <c r="F39" s="16"/>
     </row>
-    <row r="40" spans="1:6">
-      <c r="A40" s="7" t="s">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A40" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="B40" s="7" t="s">
+      <c r="B40" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="C40" s="7" t="s">
+      <c r="C40" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="D40" s="7" t="s">
+      <c r="D40" s="3" t="s">
         <v>195</v>
       </c>
-      <c r="E40" s="7" t="s">
+      <c r="E40" s="3" t="s">
         <v>180</v>
       </c>
       <c r="F40" s="16"/>
     </row>
-    <row r="41" spans="1:6">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="7" t="s">
         <v>149</v>
       </c>
@@ -2084,7 +2084,7 @@
       </c>
       <c r="F41" s="16"/>
     </row>
-    <row r="42" spans="1:6">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
         <v>154</v>
       </c>
@@ -2099,7 +2099,7 @@
       </c>
       <c r="F42" s="16"/>
     </row>
-    <row r="43" spans="1:6">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
         <v>150</v>
       </c>
@@ -2117,25 +2117,25 @@
       </c>
       <c r="F43" s="16"/>
     </row>
-    <row r="44" spans="1:6">
-      <c r="A44" s="7" t="s">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A44" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="B44" s="7" t="s">
+      <c r="B44" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="C44" s="7" t="s">
+      <c r="C44" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="D44" s="7" t="s">
+      <c r="D44" s="3" t="s">
         <v>199</v>
       </c>
-      <c r="E44" s="7" t="s">
+      <c r="E44" s="3" t="s">
         <v>184</v>
       </c>
       <c r="F44" s="16"/>
     </row>
-    <row r="45" spans="1:6">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" s="16"/>
       <c r="B45" s="7" t="s">
         <v>128</v>
@@ -2145,7 +2145,7 @@
       <c r="E45" s="16"/>
       <c r="F45" s="16"/>
     </row>
-    <row r="46" spans="1:6">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" s="16"/>
       <c r="B46" s="7" t="s">
         <v>129</v>
@@ -2155,7 +2155,7 @@
       <c r="E46" s="16"/>
       <c r="F46" s="16"/>
     </row>
-    <row r="47" spans="1:6">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" s="16"/>
       <c r="B47" s="16"/>
       <c r="C47" s="16"/>
@@ -2165,7 +2165,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="48" spans="1:6">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" s="16"/>
       <c r="B48" s="16"/>
       <c r="C48" s="16"/>
@@ -2175,7 +2175,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="49" spans="1:8">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" s="17"/>
       <c r="B49" s="17"/>
       <c r="C49" s="17"/>
@@ -2184,7 +2184,7 @@
       <c r="F49" s="17"/>
       <c r="H49" s="17"/>
     </row>
-    <row r="50" spans="1:8">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" s="17"/>
       <c r="B50" s="17"/>
       <c r="C50" s="17"/>
@@ -2193,7 +2193,7 @@
       <c r="F50" s="17"/>
       <c r="H50" s="17"/>
     </row>
-    <row r="51" spans="1:8">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" s="17"/>
       <c r="B51" s="17"/>
       <c r="C51" s="17"/>
@@ -2202,7 +2202,7 @@
       <c r="F51" s="17"/>
       <c r="H51" s="17"/>
     </row>
-    <row r="52" spans="1:8">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" s="17"/>
       <c r="B52" s="17"/>
       <c r="C52" s="17"/>
@@ -2211,7 +2211,7 @@
       <c r="F52" s="17"/>
       <c r="H52" s="17"/>
     </row>
-    <row r="53" spans="1:8">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" s="17"/>
       <c r="B53" s="17"/>
       <c r="C53" s="17"/>
@@ -2220,7 +2220,7 @@
       <c r="F53" s="17"/>
       <c r="H53" s="17"/>
     </row>
-    <row r="54" spans="1:8">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" s="17"/>
       <c r="B54" s="17"/>
       <c r="C54" s="17"/>
@@ -2229,7 +2229,7 @@
       <c r="F54" s="17"/>
       <c r="H54" s="17"/>
     </row>
-    <row r="55" spans="1:8">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" s="17"/>
       <c r="B55" s="17"/>
       <c r="C55" s="17"/>
@@ -2238,7 +2238,7 @@
       <c r="F55" s="17"/>
       <c r="H55" s="17"/>
     </row>
-    <row r="56" spans="1:8">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" s="17"/>
       <c r="B56" s="17"/>
       <c r="C56" s="17"/>
@@ -2247,7 +2247,7 @@
       <c r="F56" s="17"/>
       <c r="H56" s="17"/>
     </row>
-    <row r="57" spans="1:8">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" s="17"/>
       <c r="B57" s="17"/>
       <c r="C57" s="17"/>
@@ -2256,7 +2256,7 @@
       <c r="F57" s="17"/>
       <c r="H57" s="17"/>
     </row>
-    <row r="58" spans="1:8">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" s="17"/>
       <c r="B58" s="17"/>
       <c r="C58" s="17"/>
@@ -2265,7 +2265,7 @@
       <c r="F58" s="17"/>
       <c r="H58" s="17"/>
     </row>
-    <row r="59" spans="1:8">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59" s="17"/>
       <c r="B59" s="17"/>
       <c r="C59" s="17"/>
@@ -2274,7 +2274,7 @@
       <c r="F59" s="17"/>
       <c r="H59" s="17"/>
     </row>
-    <row r="60" spans="1:8">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A60" s="17"/>
       <c r="B60" s="17"/>
       <c r="C60" s="17"/>
@@ -2283,7 +2283,7 @@
       <c r="F60" s="17"/>
       <c r="H60" s="17"/>
     </row>
-    <row r="61" spans="1:8">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A61" s="17"/>
       <c r="B61" s="17"/>
       <c r="C61" s="17"/>
@@ -2292,7 +2292,7 @@
       <c r="F61" s="17"/>
       <c r="H61" s="17"/>
     </row>
-    <row r="62" spans="1:8">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A62" s="17"/>
       <c r="B62" s="17"/>
       <c r="C62" s="17"/>
@@ -2301,7 +2301,7 @@
       <c r="F62" s="17"/>
       <c r="H62" s="17"/>
     </row>
-    <row r="63" spans="1:8">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A63" s="17"/>
       <c r="B63" s="17"/>
       <c r="C63" s="17"/>
@@ -2310,7 +2310,7 @@
       <c r="F63" s="17"/>
       <c r="H63" s="17"/>
     </row>
-    <row r="64" spans="1:8">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A64" s="17"/>
       <c r="B64" s="17"/>
       <c r="C64" s="17"/>
@@ -2319,7 +2319,7 @@
       <c r="F64" s="17"/>
       <c r="H64" s="17"/>
     </row>
-    <row r="65" spans="1:8">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A65" s="17"/>
       <c r="B65" s="17"/>
       <c r="C65" s="17"/>
@@ -2328,7 +2328,7 @@
       <c r="F65" s="17"/>
       <c r="H65" s="17"/>
     </row>
-    <row r="66" spans="1:8">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A66" s="17"/>
       <c r="B66" s="17"/>
       <c r="C66" s="17"/>
@@ -2337,7 +2337,7 @@
       <c r="F66" s="17"/>
       <c r="H66" s="17"/>
     </row>
-    <row r="67" spans="1:8">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A67" s="17"/>
       <c r="B67" s="17"/>
       <c r="C67" s="17"/>
@@ -2346,7 +2346,7 @@
       <c r="F67" s="17"/>
       <c r="H67" s="17"/>
     </row>
-    <row r="68" spans="1:8">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A68" s="17"/>
       <c r="B68" s="17"/>
       <c r="C68" s="17"/>
@@ -2355,7 +2355,7 @@
       <c r="F68" s="17"/>
       <c r="H68" s="17"/>
     </row>
-    <row r="69" spans="1:8">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A69" s="17"/>
       <c r="B69" s="17"/>
       <c r="C69" s="17"/>
@@ -2364,7 +2364,7 @@
       <c r="F69" s="17"/>
       <c r="H69" s="17"/>
     </row>
-    <row r="70" spans="1:8">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A70" s="17"/>
       <c r="B70" s="17"/>
       <c r="C70" s="17"/>
@@ -2373,7 +2373,7 @@
       <c r="F70" s="17"/>
       <c r="H70" s="17"/>
     </row>
-    <row r="71" spans="1:8">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A71" s="17"/>
       <c r="B71" s="17"/>
       <c r="C71" s="17"/>
@@ -2382,7 +2382,7 @@
       <c r="F71" s="17"/>
       <c r="H71" s="17"/>
     </row>
-    <row r="72" spans="1:8">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A72" s="17"/>
       <c r="B72" s="17"/>
       <c r="C72" s="17"/>
@@ -2391,7 +2391,7 @@
       <c r="F72" s="17"/>
       <c r="H72" s="17"/>
     </row>
-    <row r="73" spans="1:8">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A73" s="17"/>
       <c r="B73" s="17"/>
       <c r="C73" s="17"/>
@@ -2400,7 +2400,7 @@
       <c r="F73" s="17"/>
       <c r="H73" s="17"/>
     </row>
-    <row r="74" spans="1:8">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A74" s="17"/>
       <c r="B74" s="17"/>
       <c r="C74" s="17"/>
@@ -2409,7 +2409,7 @@
       <c r="F74" s="17"/>
       <c r="H74" s="17"/>
     </row>
-    <row r="75" spans="1:8">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A75" s="17"/>
       <c r="B75" s="17"/>
       <c r="C75" s="17"/>
@@ -2418,7 +2418,7 @@
       <c r="F75" s="17"/>
       <c r="H75" s="17"/>
     </row>
-    <row r="76" spans="1:8">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A76" s="17"/>
       <c r="B76" s="17"/>
       <c r="C76" s="17"/>
@@ -2427,7 +2427,7 @@
       <c r="F76" s="17"/>
       <c r="H76" s="17"/>
     </row>
-    <row r="77" spans="1:8">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A77" s="17"/>
       <c r="B77" s="17"/>
       <c r="C77" s="17"/>
@@ -2436,7 +2436,7 @@
       <c r="F77" s="17"/>
       <c r="H77" s="17"/>
     </row>
-    <row r="78" spans="1:8">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A78" s="17"/>
       <c r="B78" s="17"/>
       <c r="C78" s="17"/>
@@ -2445,7 +2445,7 @@
       <c r="F78" s="17"/>
       <c r="H78" s="17"/>
     </row>
-    <row r="79" spans="1:8">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A79" s="17"/>
       <c r="B79" s="17"/>
       <c r="C79" s="17"/>
@@ -2454,7 +2454,7 @@
       <c r="F79" s="17"/>
       <c r="H79" s="17"/>
     </row>
-    <row r="80" spans="1:8">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A80" s="17"/>
       <c r="B80" s="17"/>
       <c r="C80" s="17"/>
@@ -2463,7 +2463,7 @@
       <c r="F80" s="17"/>
       <c r="H80" s="17"/>
     </row>
-    <row r="81" spans="1:8">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A81" s="17"/>
       <c r="B81" s="17"/>
       <c r="C81" s="17"/>
@@ -2472,7 +2472,7 @@
       <c r="F81" s="17"/>
       <c r="H81" s="17"/>
     </row>
-    <row r="82" spans="1:8">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A82" s="17"/>
       <c r="B82" s="17"/>
       <c r="C82" s="17"/>
@@ -2481,7 +2481,7 @@
       <c r="F82" s="17"/>
       <c r="H82" s="17"/>
     </row>
-    <row r="83" spans="1:8">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A83" s="17"/>
       <c r="B83" s="17"/>
       <c r="C83" s="17"/>
@@ -2490,7 +2490,7 @@
       <c r="F83" s="17"/>
       <c r="H83" s="17"/>
     </row>
-    <row r="84" spans="1:8">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A84" s="17"/>
       <c r="B84" s="17"/>
       <c r="C84" s="17"/>
@@ -2499,7 +2499,7 @@
       <c r="F84" s="17"/>
       <c r="H84" s="17"/>
     </row>
-    <row r="85" spans="1:8">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A85" s="17"/>
       <c r="B85" s="17"/>
       <c r="C85" s="17"/>
@@ -2508,7 +2508,7 @@
       <c r="F85" s="17"/>
       <c r="H85" s="17"/>
     </row>
-    <row r="86" spans="1:8">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A86" s="17"/>
       <c r="B86" s="17"/>
       <c r="C86" s="17"/>
@@ -2517,7 +2517,7 @@
       <c r="F86" s="17"/>
       <c r="H86" s="17"/>
     </row>
-    <row r="87" spans="1:8">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A87" s="17"/>
       <c r="B87" s="17"/>
       <c r="C87" s="17"/>
@@ -2526,7 +2526,7 @@
       <c r="F87" s="17"/>
       <c r="H87" s="17"/>
     </row>
-    <row r="88" spans="1:8">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A88" s="17"/>
       <c r="B88" s="17"/>
       <c r="C88" s="17"/>
@@ -2535,7 +2535,7 @@
       <c r="F88" s="17"/>
       <c r="H88" s="17"/>
     </row>
-    <row r="89" spans="1:8">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A89" s="17"/>
       <c r="B89" s="17"/>
       <c r="C89" s="17"/>
@@ -2544,7 +2544,7 @@
       <c r="F89" s="17"/>
       <c r="H89" s="17"/>
     </row>
-    <row r="90" spans="1:8">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A90" s="17"/>
       <c r="B90" s="17"/>
       <c r="C90" s="17"/>
@@ -2553,7 +2553,7 @@
       <c r="F90" s="17"/>
       <c r="H90" s="17"/>
     </row>
-    <row r="91" spans="1:8">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A91" s="17"/>
       <c r="B91" s="17"/>
       <c r="C91" s="17"/>
@@ -2562,7 +2562,7 @@
       <c r="F91" s="17"/>
       <c r="H91" s="17"/>
     </row>
-    <row r="92" spans="1:8">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A92" s="17"/>
       <c r="B92" s="17"/>
       <c r="C92" s="17"/>
@@ -2571,7 +2571,7 @@
       <c r="F92" s="17"/>
       <c r="H92" s="17"/>
     </row>
-    <row r="93" spans="1:8">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A93" s="17"/>
       <c r="B93" s="17"/>
       <c r="C93" s="17"/>
@@ -2580,7 +2580,7 @@
       <c r="F93" s="17"/>
       <c r="H93" s="17"/>
     </row>
-    <row r="94" spans="1:8">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A94" s="17"/>
       <c r="B94" s="17"/>
       <c r="C94" s="17"/>
@@ -2589,7 +2589,7 @@
       <c r="F94" s="17"/>
       <c r="H94" s="17"/>
     </row>
-    <row r="95" spans="1:8">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A95" s="17"/>
       <c r="B95" s="17"/>
       <c r="C95" s="17"/>
@@ -2598,7 +2598,7 @@
       <c r="F95" s="17"/>
       <c r="H95" s="17"/>
     </row>
-    <row r="96" spans="1:8">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A96" s="17"/>
       <c r="B96" s="17"/>
       <c r="C96" s="17"/>
@@ -2607,7 +2607,7 @@
       <c r="F96" s="17"/>
       <c r="H96" s="17"/>
     </row>
-    <row r="97" spans="1:8">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A97" s="17"/>
       <c r="B97" s="17"/>
       <c r="C97" s="17"/>
@@ -2616,7 +2616,7 @@
       <c r="F97" s="17"/>
       <c r="H97" s="17"/>
     </row>
-    <row r="98" spans="1:8">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A98" s="17"/>
       <c r="B98" s="17"/>
       <c r="C98" s="17"/>
@@ -2625,7 +2625,7 @@
       <c r="F98" s="17"/>
       <c r="H98" s="17"/>
     </row>
-    <row r="99" spans="1:8">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A99" s="17"/>
       <c r="B99" s="17"/>
       <c r="C99" s="17"/>
@@ -2634,7 +2634,7 @@
       <c r="F99" s="17"/>
       <c r="H99" s="17"/>
     </row>
-    <row r="100" spans="1:8">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A100" s="17"/>
       <c r="B100" s="17"/>
       <c r="C100" s="17"/>
@@ -2643,7 +2643,7 @@
       <c r="F100" s="17"/>
       <c r="H100" s="17"/>
     </row>
-    <row r="101" spans="1:8">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A101" s="17"/>
       <c r="B101" s="17"/>
       <c r="C101" s="17"/>
@@ -2652,7 +2652,7 @@
       <c r="F101" s="17"/>
       <c r="H101" s="17"/>
     </row>
-    <row r="102" spans="1:8">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A102" s="17"/>
       <c r="B102" s="17"/>
       <c r="C102" s="17"/>
@@ -2661,7 +2661,7 @@
       <c r="F102" s="17"/>
       <c r="H102" s="17"/>
     </row>
-    <row r="103" spans="1:8">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A103" s="17"/>
       <c r="B103" s="17"/>
       <c r="C103" s="17"/>
@@ -2670,7 +2670,7 @@
       <c r="F103" s="17"/>
       <c r="H103" s="17"/>
     </row>
-    <row r="104" spans="1:8">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A104" s="17"/>
       <c r="B104" s="17"/>
       <c r="C104" s="17"/>
@@ -2679,7 +2679,7 @@
       <c r="F104" s="17"/>
       <c r="H104" s="17"/>
     </row>
-    <row r="105" spans="1:8">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A105" s="17"/>
       <c r="B105" s="17"/>
       <c r="C105" s="17"/>
@@ -2688,7 +2688,7 @@
       <c r="F105" s="17"/>
       <c r="H105" s="17"/>
     </row>
-    <row r="106" spans="1:8">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A106" s="17"/>
       <c r="B106" s="17"/>
       <c r="C106" s="17"/>
@@ -2697,7 +2697,7 @@
       <c r="F106" s="17"/>
       <c r="H106" s="17"/>
     </row>
-    <row r="107" spans="1:8">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A107" s="17"/>
       <c r="B107" s="17"/>
       <c r="C107" s="17"/>
@@ -2706,7 +2706,7 @@
       <c r="F107" s="17"/>
       <c r="H107" s="17"/>
     </row>
-    <row r="108" spans="1:8">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A108" s="17"/>
       <c r="B108" s="17"/>
       <c r="C108" s="17"/>
@@ -2715,7 +2715,7 @@
       <c r="F108" s="17"/>
       <c r="H108" s="17"/>
     </row>
-    <row r="109" spans="1:8">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A109" s="17"/>
       <c r="B109" s="17"/>
       <c r="C109" s="17"/>
@@ -2724,7 +2724,7 @@
       <c r="F109" s="17"/>
       <c r="H109" s="17"/>
     </row>
-    <row r="110" spans="1:8">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A110" s="17"/>
       <c r="B110" s="17"/>
       <c r="C110" s="17"/>
@@ -2733,7 +2733,7 @@
       <c r="F110" s="17"/>
       <c r="H110" s="17"/>
     </row>
-    <row r="111" spans="1:8">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A111" s="17"/>
       <c r="B111" s="17"/>
       <c r="C111" s="17"/>
@@ -2742,7 +2742,7 @@
       <c r="F111" s="17"/>
       <c r="H111" s="17"/>
     </row>
-    <row r="112" spans="1:8">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A112" s="17"/>
       <c r="B112" s="17"/>
       <c r="C112" s="17"/>
@@ -2751,7 +2751,7 @@
       <c r="F112" s="17"/>
       <c r="H112" s="17"/>
     </row>
-    <row r="113" spans="1:8">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A113" s="17"/>
       <c r="B113" s="17"/>
       <c r="C113" s="17"/>
@@ -2760,7 +2760,7 @@
       <c r="F113" s="17"/>
       <c r="H113" s="17"/>
     </row>
-    <row r="114" spans="1:8">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A114" s="17"/>
       <c r="B114" s="17"/>
       <c r="C114" s="17"/>
@@ -2769,7 +2769,7 @@
       <c r="F114" s="17"/>
       <c r="H114" s="17"/>
     </row>
-    <row r="115" spans="1:8">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A115" s="17"/>
       <c r="B115" s="17"/>
       <c r="C115" s="17"/>
@@ -2778,7 +2778,7 @@
       <c r="F115" s="17"/>
       <c r="H115" s="17"/>
     </row>
-    <row r="116" spans="1:8">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A116" s="17"/>
       <c r="B116" s="17"/>
       <c r="C116" s="17"/>
@@ -2787,7 +2787,7 @@
       <c r="F116" s="17"/>
       <c r="H116" s="17"/>
     </row>
-    <row r="117" spans="1:8">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A117" s="17"/>
       <c r="B117" s="17"/>
       <c r="C117" s="17"/>
@@ -2796,7 +2796,7 @@
       <c r="F117" s="17"/>
       <c r="H117" s="17"/>
     </row>
-    <row r="118" spans="1:8">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A118" s="17"/>
       <c r="B118" s="17"/>
       <c r="C118" s="17"/>
@@ -2805,7 +2805,7 @@
       <c r="F118" s="17"/>
       <c r="H118" s="17"/>
     </row>
-    <row r="119" spans="1:8">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A119" s="17"/>
       <c r="B119" s="17"/>
       <c r="C119" s="17"/>
@@ -2814,7 +2814,7 @@
       <c r="F119" s="17"/>
       <c r="H119" s="17"/>
     </row>
-    <row r="120" spans="1:8">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A120" s="17"/>
       <c r="B120" s="17"/>
       <c r="C120" s="17"/>
@@ -2823,7 +2823,7 @@
       <c r="F120" s="17"/>
       <c r="H120" s="17"/>
     </row>
-    <row r="121" spans="1:8">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A121" s="17"/>
       <c r="B121" s="17"/>
       <c r="C121" s="17"/>
@@ -2832,7 +2832,7 @@
       <c r="F121" s="17"/>
       <c r="H121" s="17"/>
     </row>
-    <row r="122" spans="1:8">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A122" s="17"/>
       <c r="B122" s="17"/>
       <c r="C122" s="17"/>
@@ -2841,7 +2841,7 @@
       <c r="F122" s="17"/>
       <c r="H122" s="17"/>
     </row>
-    <row r="123" spans="1:8">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A123" s="17"/>
       <c r="B123" s="17"/>
       <c r="C123" s="17"/>
@@ -2866,7 +2866,7 @@
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="61.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.75" bestFit="1" customWidth="1"/>
@@ -2875,7 +2875,7 @@
     <col min="5" max="5" width="6.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>124</v>
       </c>
@@ -2889,7 +2889,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>125</v>
       </c>
@@ -2905,7 +2905,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>126</v>
       </c>
@@ -2921,7 +2921,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>127</v>
       </c>
@@ -2937,7 +2937,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>128</v>
       </c>
@@ -2953,7 +2953,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>129</v>
       </c>
@@ -2969,7 +2969,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>130</v>
       </c>
@@ -2985,7 +2985,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>131</v>
       </c>
@@ -3001,7 +3001,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>132</v>
       </c>
@@ -3017,7 +3017,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>133</v>
       </c>
@@ -3033,7 +3033,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>134</v>
       </c>
@@ -3049,7 +3049,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>135</v>
       </c>
@@ -3065,7 +3065,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>136</v>
       </c>
@@ -3081,7 +3081,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>137</v>
       </c>
@@ -3097,7 +3097,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>138</v>
       </c>
@@ -3113,7 +3113,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>140</v>
       </c>
@@ -3129,7 +3129,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>139</v>
       </c>
@@ -3145,7 +3145,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>141</v>
       </c>
@@ -3161,7 +3161,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>142</v>
       </c>
@@ -3177,7 +3177,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>143</v>
       </c>
@@ -3193,7 +3193,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>146</v>
       </c>
@@ -3209,7 +3209,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>144</v>
       </c>
@@ -3225,7 +3225,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>145</v>
       </c>
@@ -3241,7 +3241,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>147</v>
       </c>
@@ -3257,7 +3257,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>148</v>
       </c>
@@ -3273,7 +3273,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>149</v>
       </c>
@@ -3289,7 +3289,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>150</v>
       </c>
@@ -3305,7 +3305,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>151</v>
       </c>
@@ -3321,7 +3321,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>152</v>
       </c>
@@ -3337,7 +3337,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>153</v>
       </c>
@@ -3353,7 +3353,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="31" spans="1:5">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>154</v>
       </c>
@@ -3369,7 +3369,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>0</v>
       </c>
@@ -3385,7 +3385,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>1</v>
       </c>
@@ -3401,7 +3401,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>2</v>
       </c>
@@ -3417,7 +3417,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="35" spans="1:5">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>3</v>
       </c>
@@ -3433,7 +3433,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="36" spans="1:5">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>4</v>
       </c>
@@ -3449,7 +3449,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="37" spans="1:5">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>5</v>
       </c>
@@ -3465,7 +3465,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="38" spans="1:5">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>6</v>
       </c>
@@ -3481,7 +3481,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="39" spans="1:5">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>7</v>
       </c>
@@ -3497,7 +3497,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="40" spans="1:5">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>8</v>
       </c>
@@ -3513,7 +3513,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="41" spans="1:5">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>9</v>
       </c>
@@ -3529,7 +3529,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="42" spans="1:5">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>10</v>
       </c>
@@ -3545,7 +3545,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="43" spans="1:5">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>11</v>
       </c>
@@ -3561,7 +3561,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="44" spans="1:5">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>14</v>
       </c>
@@ -3577,7 +3577,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="45" spans="1:5">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>12</v>
       </c>
@@ -3593,7 +3593,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="46" spans="1:5">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>13</v>
       </c>
@@ -3609,7 +3609,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="47" spans="1:5">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>16</v>
       </c>
@@ -3625,7 +3625,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="48" spans="1:5">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>17</v>
       </c>
@@ -3641,7 +3641,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="49" spans="1:5">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>19</v>
       </c>
@@ -3657,7 +3657,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="50" spans="1:5">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>20</v>
       </c>
@@ -3673,7 +3673,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="51" spans="1:5">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>21</v>
       </c>
@@ -3689,7 +3689,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="52" spans="1:5">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>22</v>
       </c>
@@ -3705,7 +3705,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="53" spans="1:5">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>23</v>
       </c>
@@ -3721,7 +3721,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="54" spans="1:5">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>24</v>
       </c>
@@ -3737,7 +3737,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="55" spans="1:5">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>25</v>
       </c>
@@ -3753,7 +3753,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="56" spans="1:5">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>26</v>
       </c>
@@ -3769,7 +3769,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="57" spans="1:5">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>27</v>
       </c>
@@ -3785,7 +3785,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="58" spans="1:5">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>28</v>
       </c>
@@ -3801,7 +3801,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="59" spans="1:5">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>29</v>
       </c>
@@ -3817,7 +3817,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="60" spans="1:5">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>30</v>
       </c>
@@ -3833,7 +3833,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="61" spans="1:5">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>31</v>
       </c>
@@ -3849,7 +3849,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="62" spans="1:5">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>32</v>
       </c>
@@ -3865,7 +3865,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="63" spans="1:5">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>33</v>
       </c>
@@ -3881,7 +3881,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="64" spans="1:5">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>34</v>
       </c>
@@ -3897,7 +3897,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="65" spans="1:5">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>36</v>
       </c>
@@ -3913,7 +3913,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="66" spans="1:5">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>35</v>
       </c>
@@ -3929,7 +3929,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="67" spans="1:5">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>37</v>
       </c>
@@ -3945,7 +3945,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="68" spans="1:5">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>38</v>
       </c>
@@ -3961,7 +3961,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="69" spans="1:5">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>39</v>
       </c>
@@ -3977,7 +3977,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="70" spans="1:5">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>40</v>
       </c>
@@ -3993,7 +3993,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="71" spans="1:5">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D71" t="s">
         <v>65</v>
       </c>
@@ -4002,7 +4002,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="72" spans="1:5">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D72" t="s">
         <v>66</v>
       </c>
@@ -4011,7 +4011,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="73" spans="1:5">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D73" t="s">
         <v>67</v>
       </c>
@@ -4020,7 +4020,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="74" spans="1:5">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D74" t="s">
         <v>68</v>
       </c>
@@ -4029,7 +4029,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="75" spans="1:5">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D75" t="s">
         <v>69</v>
       </c>
@@ -4038,7 +4038,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="76" spans="1:5">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D76" t="s">
         <v>70</v>
       </c>
@@ -4047,7 +4047,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="77" spans="1:5">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D77" t="s">
         <v>71</v>
       </c>
@@ -4056,7 +4056,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="78" spans="1:5">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D78" t="s">
         <v>72</v>
       </c>
@@ -4065,7 +4065,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="79" spans="1:5">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D79" t="s">
         <v>73</v>
       </c>
@@ -4074,7 +4074,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="80" spans="1:5">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D80" t="s">
         <v>74</v>
       </c>
@@ -4083,7 +4083,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="81" spans="4:5">
+    <row r="81" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D81" t="s">
         <v>75</v>
       </c>
@@ -4092,7 +4092,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="82" spans="4:5">
+    <row r="82" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D82" t="s">
         <v>76</v>
       </c>
@@ -4101,7 +4101,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="83" spans="4:5">
+    <row r="83" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D83" t="s">
         <v>77</v>
       </c>
@@ -4110,7 +4110,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="84" spans="4:5">
+    <row r="84" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D84" t="s">
         <v>78</v>
       </c>
@@ -4119,7 +4119,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="85" spans="4:5">
+    <row r="85" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D85" t="s">
         <v>79</v>
       </c>
@@ -4128,7 +4128,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="86" spans="4:5">
+    <row r="86" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D86" t="s">
         <v>80</v>
       </c>
@@ -4137,7 +4137,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="87" spans="4:5">
+    <row r="87" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D87" t="s">
         <v>81</v>
       </c>
@@ -4146,7 +4146,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="88" spans="4:5">
+    <row r="88" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D88" t="s">
         <v>82</v>
       </c>
@@ -4155,7 +4155,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="89" spans="4:5">
+    <row r="89" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D89" t="s">
         <v>83</v>
       </c>
@@ -4164,7 +4164,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="90" spans="4:5">
+    <row r="90" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D90" t="s">
         <v>84</v>
       </c>
@@ -4173,7 +4173,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="91" spans="4:5">
+    <row r="91" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D91" t="s">
         <v>85</v>
       </c>
@@ -4182,7 +4182,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="92" spans="4:5">
+    <row r="92" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D92" t="s">
         <v>86</v>
       </c>
@@ -4191,7 +4191,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="93" spans="4:5">
+    <row r="93" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D93" t="s">
         <v>87</v>
       </c>
@@ -4200,7 +4200,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="94" spans="4:5">
+    <row r="94" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D94" t="s">
         <v>88</v>
       </c>
@@ -4209,7 +4209,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="95" spans="4:5">
+    <row r="95" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D95" t="s">
         <v>89</v>
       </c>
@@ -4218,7 +4218,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="96" spans="4:5">
+    <row r="96" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D96" t="s">
         <v>90</v>
       </c>
@@ -4227,7 +4227,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="97" spans="4:5">
+    <row r="97" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D97" t="s">
         <v>91</v>
       </c>
@@ -4236,7 +4236,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="98" spans="4:5">
+    <row r="98" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D98" t="s">
         <v>92</v>
       </c>
@@ -4245,7 +4245,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="99" spans="4:5">
+    <row r="99" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D99" t="s">
         <v>93</v>
       </c>
@@ -4254,7 +4254,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="100" spans="4:5">
+    <row r="100" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D100" t="s">
         <v>94</v>
       </c>
@@ -4263,7 +4263,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="101" spans="4:5">
+    <row r="101" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D101" t="s">
         <v>95</v>
       </c>
@@ -4272,7 +4272,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="102" spans="4:5">
+    <row r="102" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D102" t="s">
         <v>96</v>
       </c>
@@ -4281,7 +4281,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="103" spans="4:5">
+    <row r="103" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D103" t="s">
         <v>97</v>
       </c>
@@ -4290,7 +4290,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="104" spans="4:5">
+    <row r="104" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D104" t="s">
         <v>98</v>
       </c>
@@ -4299,7 +4299,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="105" spans="4:5">
+    <row r="105" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D105" t="s">
         <v>99</v>
       </c>
@@ -4308,7 +4308,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="106" spans="4:5">
+    <row r="106" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D106" t="s">
         <v>100</v>
       </c>
@@ -4317,7 +4317,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="107" spans="4:5">
+    <row r="107" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D107" t="s">
         <v>101</v>
       </c>
@@ -4326,7 +4326,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="108" spans="4:5">
+    <row r="108" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D108" t="s">
         <v>102</v>
       </c>
@@ -4335,7 +4335,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="109" spans="4:5">
+    <row r="109" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D109" t="s">
         <v>103</v>
       </c>
@@ -4344,7 +4344,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="110" spans="4:5">
+    <row r="110" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D110" t="s">
         <v>104</v>
       </c>
@@ -4353,7 +4353,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="111" spans="4:5">
+    <row r="111" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D111" t="s">
         <v>105</v>
       </c>
@@ -4362,7 +4362,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="112" spans="4:5">
+    <row r="112" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D112" t="s">
         <v>106</v>
       </c>
@@ -4371,7 +4371,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="113" spans="4:5">
+    <row r="113" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D113" t="s">
         <v>107</v>
       </c>
@@ -4380,7 +4380,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="114" spans="4:5">
+    <row r="114" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D114" t="s">
         <v>108</v>
       </c>
@@ -4389,7 +4389,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="115" spans="4:5">
+    <row r="115" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D115" t="s">
         <v>109</v>
       </c>
@@ -4398,7 +4398,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="116" spans="4:5">
+    <row r="116" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D116" t="s">
         <v>110</v>
       </c>
@@ -4407,7 +4407,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="117" spans="4:5">
+    <row r="117" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D117" t="s">
         <v>111</v>
       </c>
@@ -4416,7 +4416,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="118" spans="4:5">
+    <row r="118" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D118" t="s">
         <v>112</v>
       </c>
@@ -4425,7 +4425,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="119" spans="4:5">
+    <row r="119" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D119" t="s">
         <v>113</v>
       </c>
@@ -4434,7 +4434,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="120" spans="4:5">
+    <row r="120" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D120" t="s">
         <v>114</v>
       </c>
@@ -4443,7 +4443,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="121" spans="4:5">
+    <row r="121" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D121" t="s">
         <v>115</v>
       </c>
@@ -4452,7 +4452,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="122" spans="4:5">
+    <row r="122" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D122" t="s">
         <v>116</v>
       </c>
@@ -4461,7 +4461,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="123" spans="4:5">
+    <row r="123" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D123" t="s">
         <v>117</v>
       </c>
@@ -4470,7 +4470,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="124" spans="4:5">
+    <row r="124" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D124" t="s">
         <v>118</v>
       </c>

</xml_diff>

<commit_message>
tipo almacen, cotixacion. cotizacion Recurros, 3 APIS añadidas
</commit_message>
<xml_diff>
--- a/QuerysAñadidas.xlsx
+++ b/QuerysAñadidas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ncano\Desktop\inacons-frontend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BB4E110-F79F-4ED6-AFAB-6D99AE66E964}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B64D84B-1B0A-4BBD-A416-E8A628F5B4C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C2939682-D91A-4BD3-AD71-BB0CA9127A74}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="216">
   <si>
     <t>getAllUsuarios:[Usuario]</t>
   </si>
@@ -418,33 +418,18 @@
     <t>getCotizacionRecurso(…):CotizacionRecurso</t>
   </si>
   <si>
-    <t>getCotizacionRecursoforCotizacionId(…):</t>
-  </si>
-  <si>
     <t>getOrdenCompraRecursoforOrdenId(…):[OrdenCompraRecurso!]!</t>
   </si>
   <si>
     <t>getOrdenSolicitudRecursoforSolicitudId(…):</t>
   </si>
   <si>
-    <t>getRequerimientoAbrobacionbyRequerimientoId(…):</t>
-  </si>
-  <si>
     <t>getRequerimientoRecursoByRequerimientoId(…):</t>
   </si>
   <si>
-    <t>getRequerimientoRecursoByRequerimientoIdWithAlmacenQuantities(…):</t>
-  </si>
-  <si>
     <t>listAlmacenCentroCostos:[AlmacenCentroCosto!]!</t>
   </si>
   <si>
-    <t>listAlmacenCentroCostosByAlmacenId(…):</t>
-  </si>
-  <si>
-    <t>listAlmacenCentroCostosByCentroCostoId(…):</t>
-  </si>
-  <si>
     <t>listBodegas:[Bodega!]!</t>
   </si>
   <si>
@@ -454,9 +439,6 @@
     <t>listClasificacionRecursoByParentId(…):</t>
   </si>
   <si>
-    <t>listCotizacionRecursos:[CotizacionRecurso!]!</t>
-  </si>
-  <si>
     <t>listCotizaciones:[Cotizacion!]!</t>
   </si>
   <si>
@@ -514,9 +496,6 @@
     <t>addCotizacion(…):Cotizacion!</t>
   </si>
   <si>
-    <t>addCotizacionRecurso(…):CotizacionRecurso!</t>
-  </si>
-  <si>
     <t>addGuiaTransferencia(…):GuiaTransferencia!</t>
   </si>
   <si>
@@ -644,13 +623,73 @@
   </si>
   <si>
     <t>Adicional</t>
+  </si>
+  <si>
+    <t>findPreSolicitudByRequerimiento(…):[PreSolicitudAlmacenDetallada!]!</t>
+  </si>
+  <si>
+    <t>getCotizacionRecursoforCotizacionId(…):[CotizacionRecurso!]!</t>
+  </si>
+  <si>
+    <t>getCotizacionRecursoforCotizacionIdv(…):[CotizacionRecurso!]!</t>
+  </si>
+  <si>
+    <t>getCotizacionRecursov(…):CotizacionRecurso</t>
+  </si>
+  <si>
+    <t>getOrdenSolicitudRecursoforSolicitudId(…):[SolicitudRecursoAlmacen!]!</t>
+  </si>
+  <si>
+    <t>getRequerimientoAbrobacionbyRequerimientoId(…):[RequerimientoAprobacion]</t>
+  </si>
+  <si>
+    <t>getRequerimientoRecursoByRequerimientoIdWithAlmacenQuantities(…):[RequerimientoRecurso!]!</t>
+  </si>
+  <si>
+    <t>listAlmacenCentroCostosByAlmacenId(…):[AlmacenCentroCosto!]!</t>
+  </si>
+  <si>
+    <t>listAlmacenCentroCostosByCentroCostoId(…):[AlmacenCentroCosto!]!</t>
+  </si>
+  <si>
+    <t>listCotizacionRecurso:[CotizacionRecurso!]!</t>
+  </si>
+  <si>
+    <t>listCotizacionRecursov:[CotizacionRecurso!]!</t>
+  </si>
+  <si>
+    <t>listGuiaTransferenciasByTransferenciaId(…):[GuiaTransferencia!]!</t>
+  </si>
+  <si>
+    <t>listPreSolicitudAlmacenRecursosByPreSolicitudId(…):[PreSolicitudAlmacenRecurso!]!</t>
+  </si>
+  <si>
+    <t>listTransferenciaDetallesByTransferenciaId(…):[TransferenciaDetalle!]!</t>
+  </si>
+  <si>
+    <t>listTransferenciaRecursosByTransferenciaDetalle(…):[TransferenciaRecurso!]!</t>
+  </si>
+  <si>
+    <t>testRolfsi:[TestRolf]</t>
+  </si>
+  <si>
+    <t>addCotizacionRecurso(…):CotizacionRecurso</t>
+  </si>
+  <si>
+    <t>addCotizacionRecursosv(…):CotizacionRecurso</t>
+  </si>
+  <si>
+    <t>deleteCotizacionRecursov(…):CotizacionRecurso</t>
+  </si>
+  <si>
+    <t>updateCotizacionRecursov(…):CotizacionRecurso</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -679,8 +718,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -729,8 +774,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor theme="4" tint="0.59999389629810485"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor theme="0" tint="-0.14999847407452621"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -762,11 +825,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -776,7 +850,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -792,21 +865,52 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="11">
+  <dxfs count="12">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFE97132"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFE97132"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -928,14 +1032,6 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFE97132"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <strike val="0"/>
         <outline val="0"/>
@@ -988,32 +1084,32 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{20C6C63B-275B-4ABF-915E-BB850EBA3796}" name="Tabla1" displayName="Tabla1" ref="A1:F48" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
-  <autoFilter ref="A1:F48" xr:uid="{20C6C63B-275B-4ABF-915E-BB850EBA3796}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F30">
-    <sortCondition sortBy="cellColor" ref="C1:C30" dxfId="8"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{20C6C63B-275B-4ABF-915E-BB850EBA3796}" name="Tabla1" displayName="Tabla1" ref="A1:F50" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:F50" xr:uid="{20C6C63B-275B-4ABF-915E-BB850EBA3796}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F50">
+    <sortCondition ref="B1:B50"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="2" xr3:uid="{9A32BBF7-304C-49E3-AE42-106F9CEEC961}" name="Listar" dataDxfId="7"/>
-    <tableColumn id="1" xr3:uid="{C011CDE6-69F6-4DE8-B5A1-2E6AF137E527}" name="Buscar por Id" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{7FF29903-9CE1-4BD7-849F-3471C53EC880}" name="Agregar" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{30FB0AF3-511C-4F53-947B-89013B98F552}" name="Actualizar" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{D1A0B2A0-09FE-47C4-9132-E8B248D6B643}" name="Borrar" dataDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{C7C99C68-6028-4378-A991-EDE5C1106AD0}" name="Adicional" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{9A32BBF7-304C-49E3-AE42-106F9CEEC961}" name="Listar" dataDxfId="9"/>
+    <tableColumn id="1" xr3:uid="{C011CDE6-69F6-4DE8-B5A1-2E6AF137E527}" name="Buscar por Id" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{7FF29903-9CE1-4BD7-849F-3471C53EC880}" name="Agregar" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{30FB0AF3-511C-4F53-947B-89013B98F552}" name="Actualizar" dataDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{D1A0B2A0-09FE-47C4-9132-E8B248D6B643}" name="Borrar" dataDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{C7C99C68-6028-4378-A991-EDE5C1106AD0}" name="Adicional" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{3DB514D5-2978-4BB5-AA4D-BEAF7ED76FD4}" name="Tabla2" displayName="Tabla2" ref="A1:B70" totalsRowShown="0">
-  <autoFilter ref="A1:B70" xr:uid="{3DB514D5-2978-4BB5-AA4D-BEAF7ED76FD4}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B70">
-    <sortCondition ref="B1:B70"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{3DB514D5-2978-4BB5-AA4D-BEAF7ED76FD4}" name="Tabla2" displayName="Tabla2" ref="A1:B75" totalsRowShown="0">
+  <autoFilter ref="A1:B75" xr:uid="{3DB514D5-2978-4BB5-AA4D-BEAF7ED76FD4}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B75">
+    <sortCondition ref="B1:B75"/>
   </sortState>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{07DF1573-2247-40CE-B621-CD9F890FEE85}" name="Fields"/>
-    <tableColumn id="2" xr3:uid="{14EB541F-AFB3-43BD-B828-03CCB6D71996}" name="Esta" dataDxfId="1">
+    <tableColumn id="2" xr3:uid="{14EB541F-AFB3-43BD-B828-03CCB6D71996}" name="Esta" dataDxfId="3">
       <calculatedColumnFormula>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1022,14 +1118,14 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{09B216DF-1195-4130-9747-41370EB84C29}" name="Tabla3" displayName="Tabla3" ref="D1:E124" totalsRowShown="0">
-  <autoFilter ref="D1:E124" xr:uid="{09B216DF-1195-4130-9747-41370EB84C29}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="D2:E124">
-    <sortCondition ref="E1:E124"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{09B216DF-1195-4130-9747-41370EB84C29}" name="Tabla3" displayName="Tabla3" ref="D1:E127" totalsRowShown="0">
+  <autoFilter ref="D1:E127" xr:uid="{09B216DF-1195-4130-9747-41370EB84C29}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="D2:E128">
+    <sortCondition ref="E1:E128"/>
   </sortState>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{0BA8BFE6-88AF-42D6-A824-7FA4D629D59D}" name="Fields"/>
-    <tableColumn id="2" xr3:uid="{34297603-D01A-4DD1-AEBB-FB24C3DD8C1E}" name="Esta" dataDxfId="0">
+    <tableColumn id="2" xr3:uid="{34297603-D01A-4DD1-AEBB-FB24C3DD8C1E}" name="Esta" dataDxfId="2">
       <calculatedColumnFormula>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1354,10 +1450,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DE2F4B0-FA8B-45A2-B9E1-1433688D7CE8}">
-  <dimension ref="A1:H123"/>
+  <dimension ref="A1:H106"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41"/>
+      <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1368,7 +1464,7 @@
     <col min="4" max="4" width="52.625" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="52.125" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="60.375" style="2" customWidth="1"/>
-    <col min="7" max="7" width="65.125" style="17" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="65.125" style="14" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11" style="2"/>
     <col min="9" max="9" width="67.125" style="2" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9.625" style="2" bestFit="1" customWidth="1"/>
@@ -1392,111 +1488,123 @@
         <v>123</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="6"/>
-      <c r="B2" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
+      <c r="A2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="B3" s="26" t="s">
+        <v>2</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>66</v>
+        <v>42</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>40</v>
+        <v>94</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>1</v>
+        <v>19</v>
+      </c>
+      <c r="B4" s="18" t="s">
+        <v>3</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>15</v>
-      </c>
+        <v>71</v>
+      </c>
+      <c r="F4" s="13"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>2</v>
+        <v>20</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>4</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>13</v>
+        <v>72</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" s="14" t="s">
-        <v>138</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>44</v>
+      <c r="A6" s="29" t="s">
+        <v>134</v>
+      </c>
+      <c r="B6" s="29" t="s">
+        <v>125</v>
+      </c>
+      <c r="C6" s="29" t="s">
+        <v>152</v>
+      </c>
+      <c r="D6" s="29" t="s">
+        <v>181</v>
+      </c>
+      <c r="E6" s="29" t="s">
+        <v>167</v>
+      </c>
+      <c r="F6" s="13"/>
+    </row>
+    <row r="7" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A7" s="18" t="s">
+        <v>205</v>
+      </c>
+      <c r="B7" s="17" t="s">
+        <v>126</v>
+      </c>
+      <c r="C7" s="30" t="s">
+        <v>212</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>18</v>
+        <v>182</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="F7" s="18" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -1515,7 +1623,7 @@
       <c r="E8" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="F8" s="16"/>
+      <c r="F8" s="13"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
@@ -1533,1322 +1641,1177 @@
       <c r="E9" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="F9" s="16"/>
+      <c r="F9" s="13"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="8" t="s">
+      <c r="A10" s="23"/>
+      <c r="B10" s="19" t="s">
+        <v>127</v>
+      </c>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+    </row>
+    <row r="11" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="23"/>
+      <c r="B11" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="C11" s="13"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="15"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="23"/>
+      <c r="B12" s="19" t="s">
+        <v>200</v>
+      </c>
+      <c r="C12" s="23"/>
+      <c r="D12" s="23"/>
+      <c r="E12" s="23"/>
+      <c r="F12" s="23"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="14" t="s">
-        <v>130</v>
-      </c>
-      <c r="C12" s="8" t="s">
+      <c r="B14" s="18" t="s">
+        <v>201</v>
+      </c>
+      <c r="C14" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="D12" s="8" t="s">
+      <c r="D14" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="E12" s="8" t="s">
+      <c r="E14" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="F12" s="9" t="s">
+      <c r="F14" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="G12" s="18"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="10" t="s">
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="B13" s="10" t="s">
+      <c r="B15" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="11" t="s">
+      <c r="C15" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="D13" s="11" t="s">
+      <c r="D15" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="E13" s="11" t="s">
+      <c r="E15" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="F13" s="12" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" s="10" t="s">
+      <c r="F15" s="11" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="B14" s="10" t="s">
+      <c r="B16" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C14" s="11" t="s">
+      <c r="C16" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="D14" s="11" t="s">
+      <c r="D16" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="E14" s="11" t="s">
+      <c r="E16" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="F14" s="12" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" s="10" t="s">
+      <c r="F16" s="11" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="B15" s="10" t="s">
+      <c r="B17" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C15" s="11" t="s">
+      <c r="C17" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="D15" s="11" t="s">
+      <c r="D17" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="E15" s="11" t="s">
+      <c r="E17" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="F15" s="12" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" s="10" t="s">
+      <c r="F17" s="11" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="B16" s="10" t="s">
+      <c r="B18" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C16" s="11" t="s">
+      <c r="C18" s="28" t="s">
         <v>56</v>
       </c>
-      <c r="D16" s="11" t="s">
+      <c r="D18" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="E16" s="11" t="s">
+      <c r="E18" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="F16" s="13" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>84</v>
+      <c r="F18" s="32" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>37</v>
+        <v>33</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
+      </c>
+      <c r="B20" s="18" t="s">
+        <v>10</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>89</v>
-      </c>
+        <v>112</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="F20" s="13"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
-        <v>39</v>
+        <v>0</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>11</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>90</v>
+        <v>91</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22" s="4" t="s">
-        <v>22</v>
+      <c r="A22" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="B22" s="18" t="s">
+        <v>203</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>99</v>
+        <v>149</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>178</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>73</v>
+        <v>164</v>
+      </c>
+      <c r="F22" s="18" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>3</v>
+        <v>17</v>
+      </c>
+      <c r="B23" s="26" t="s">
+        <v>133</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="F23" s="16"/>
+        <v>96</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
-        <v>20</v>
+        <v>135</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>4</v>
+        <v>136</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>46</v>
+        <v>153</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>98</v>
+        <v>183</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="F24" s="3" t="s">
-        <v>21</v>
-      </c>
+        <v>169</v>
+      </c>
+      <c r="F24" s="13"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B25" s="16"/>
+        <v>140</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>139</v>
+      </c>
       <c r="C25" s="3" t="s">
-        <v>49</v>
+        <v>155</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>102</v>
+        <v>186</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="F25" s="16"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+        <v>171</v>
+      </c>
+      <c r="F25" s="13"/>
+    </row>
+    <row r="26" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B26" s="16"/>
+        <v>138</v>
+      </c>
+      <c r="B26" s="31" t="s">
+        <v>208</v>
+      </c>
       <c r="C26" s="3" t="s">
-        <v>50</v>
+        <v>156</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>103</v>
+        <v>187</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="F26" s="16"/>
+        <v>172</v>
+      </c>
+      <c r="F26" s="31" t="s">
+        <v>196</v>
+      </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B27" s="16"/>
+        <v>141</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>142</v>
+      </c>
       <c r="C27" s="3" t="s">
-        <v>58</v>
+        <v>157</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>111</v>
+        <v>188</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="F27" s="16"/>
+        <v>173</v>
+      </c>
+      <c r="F27" s="13"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B28" s="16"/>
+        <v>144</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>145</v>
+      </c>
       <c r="C28" s="3" t="s">
-        <v>60</v>
+        <v>162</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>113</v>
+        <v>191</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="F28" s="16"/>
+        <v>176</v>
+      </c>
+      <c r="F28" s="13"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
-        <v>36</v>
+        <v>146</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>10</v>
+        <v>147</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>59</v>
+        <v>163</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>112</v>
+        <v>192</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="F29" s="16"/>
+        <v>177</v>
+      </c>
+      <c r="F29" s="13"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A30" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B30" s="16"/>
-      <c r="C30" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="E30" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="F30" s="16"/>
+      <c r="A30" s="24"/>
+      <c r="B30" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="C30" s="6"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="6"/>
+      <c r="F30" s="6"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>134</v>
-      </c>
+        <v>131</v>
+      </c>
+      <c r="B31" s="13"/>
       <c r="C31" s="3" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="F31" s="3" t="s">
-        <v>135</v>
-      </c>
+        <v>165</v>
+      </c>
+      <c r="F31" s="13"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="B32" s="16"/>
+        <v>16</v>
+      </c>
       <c r="C32" s="3" t="s">
-        <v>156</v>
+        <v>43</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="E32" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="F32" s="16"/>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+        <v>95</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="B33" s="13"/>
+      <c r="C33" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="F33" s="20"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A34" s="19" t="s">
+        <v>207</v>
+      </c>
+      <c r="B34" s="12" t="s">
+        <v>209</v>
+      </c>
+      <c r="C34" s="13"/>
+      <c r="D34" s="13"/>
+      <c r="E34" s="13"/>
+      <c r="F34" s="12" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A35" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A36" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="B33" s="16"/>
-      <c r="C33" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="E33" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="F33" s="16"/>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A34" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="C34" s="3" t="s">
+      <c r="B36" s="13"/>
+      <c r="C36" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="F36" s="13"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A37" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B37" s="13"/>
+      <c r="C37" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="F37" s="13"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A38" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B38" s="13"/>
+      <c r="C38" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="F38" s="13"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A39" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="E39" s="4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A40" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E40" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="F40" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A41" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B41" s="13"/>
+      <c r="C41" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="E41" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="F41" s="13"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A42" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B42" s="13"/>
+      <c r="C42" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="E42" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="F42" s="22"/>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A43" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B43" s="13"/>
+      <c r="C43" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="E43" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="F43" s="22"/>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A44" s="17" t="s">
+        <v>143</v>
+      </c>
+      <c r="B44" s="13"/>
+      <c r="C44" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="E44" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="F44" s="13"/>
+      <c r="H44" s="14"/>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A45" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="E45" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="H45" s="14"/>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A46" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="B46" s="25"/>
+      <c r="C46" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="E46" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="H46" s="14"/>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A47" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="E47" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="F47" s="23"/>
+      <c r="H47" s="14"/>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A48" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="B48" s="25"/>
+      <c r="C48" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="E48" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="H48" s="14"/>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A49" s="23"/>
+      <c r="B49" s="20"/>
+      <c r="C49" s="13"/>
+      <c r="D49" s="13"/>
+      <c r="E49" s="13"/>
+      <c r="F49" s="21" t="s">
         <v>158</v>
       </c>
-      <c r="D34" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="E34" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="F34" s="16"/>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A35" s="7" t="s">
-        <v>139</v>
-      </c>
-      <c r="B35" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="C35" s="7" t="s">
+      <c r="H49" s="14"/>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A50" s="23"/>
+      <c r="B50" s="27"/>
+      <c r="C50" s="13"/>
+      <c r="D50" s="13"/>
+      <c r="E50" s="13"/>
+      <c r="F50" s="21" t="s">
         <v>159</v>
       </c>
-      <c r="D35" s="7" t="s">
-        <v>189</v>
-      </c>
-      <c r="E35" s="7" t="s">
-        <v>175</v>
-      </c>
-      <c r="F35" s="7" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A36" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="D36" s="3" t="s">
-        <v>190</v>
-      </c>
-      <c r="E36" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="F36" s="16"/>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A37" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="B37" s="16"/>
-      <c r="C37" s="3" t="s">
-        <v>161</v>
-      </c>
-      <c r="D37" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="E37" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="F37" s="16"/>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A38" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="B38" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="D38" s="3" t="s">
-        <v>193</v>
-      </c>
-      <c r="E38" s="3" t="s">
-        <v>178</v>
-      </c>
-      <c r="F38" s="16"/>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A39" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="C39" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="D39" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="E39" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="F39" s="16"/>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A40" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="B40" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="C40" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="D40" s="3" t="s">
-        <v>195</v>
-      </c>
-      <c r="E40" s="3" t="s">
-        <v>180</v>
-      </c>
-      <c r="F40" s="16"/>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A41" s="7" t="s">
-        <v>149</v>
-      </c>
-      <c r="B41" s="16"/>
-      <c r="C41" s="7" t="s">
-        <v>167</v>
-      </c>
-      <c r="D41" s="7" t="s">
-        <v>196</v>
-      </c>
-      <c r="E41" s="7" t="s">
-        <v>181</v>
-      </c>
-      <c r="F41" s="16"/>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A42" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="C42" s="3" t="s">
-        <v>168</v>
-      </c>
-      <c r="D42" s="3" t="s">
-        <v>197</v>
-      </c>
-      <c r="E42" s="3" t="s">
-        <v>182</v>
-      </c>
-      <c r="F42" s="16"/>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A43" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="B43" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="C43" s="3" t="s">
-        <v>169</v>
-      </c>
-      <c r="D43" s="3" t="s">
-        <v>198</v>
-      </c>
-      <c r="E43" s="3" t="s">
-        <v>183</v>
-      </c>
-      <c r="F43" s="16"/>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A44" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="B44" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="C44" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="D44" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="E44" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="F44" s="16"/>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A45" s="16"/>
-      <c r="B45" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="C45" s="16"/>
-      <c r="D45" s="16"/>
-      <c r="E45" s="16"/>
-      <c r="F45" s="16"/>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A46" s="16"/>
-      <c r="B46" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="C46" s="16"/>
-      <c r="D46" s="16"/>
-      <c r="E46" s="16"/>
-      <c r="F46" s="16"/>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A47" s="16"/>
-      <c r="B47" s="16"/>
-      <c r="C47" s="16"/>
-      <c r="D47" s="16"/>
-      <c r="E47" s="16"/>
-      <c r="F47" s="15" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A48" s="16"/>
-      <c r="B48" s="16"/>
-      <c r="C48" s="16"/>
-      <c r="D48" s="16"/>
-      <c r="E48" s="16"/>
-      <c r="F48" s="15" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A49" s="17"/>
-      <c r="B49" s="17"/>
-      <c r="C49" s="17"/>
-      <c r="D49" s="17"/>
-      <c r="E49" s="17"/>
-      <c r="F49" s="17"/>
-      <c r="H49" s="17"/>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A50" s="17"/>
-      <c r="B50" s="17"/>
-      <c r="C50" s="17"/>
-      <c r="D50" s="17"/>
-      <c r="E50" s="17"/>
-      <c r="F50" s="17"/>
-      <c r="H50" s="17"/>
+      <c r="H50" s="14"/>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A51" s="17"/>
-      <c r="B51" s="17"/>
-      <c r="C51" s="17"/>
-      <c r="D51" s="17"/>
-      <c r="E51" s="17"/>
-      <c r="F51" s="17"/>
-      <c r="H51" s="17"/>
+      <c r="A51" s="14"/>
+      <c r="B51" s="14"/>
+      <c r="C51" s="14"/>
+      <c r="D51" s="14"/>
+      <c r="E51" s="14"/>
+      <c r="F51" s="14"/>
+      <c r="H51" s="14"/>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A52" s="17"/>
-      <c r="B52" s="17"/>
-      <c r="C52" s="17"/>
-      <c r="D52" s="17"/>
-      <c r="E52" s="17"/>
-      <c r="F52" s="17"/>
-      <c r="H52" s="17"/>
+      <c r="A52" s="14"/>
+      <c r="B52" s="14"/>
+      <c r="C52" s="14"/>
+      <c r="D52" s="14"/>
+      <c r="E52" s="14"/>
+      <c r="F52" s="14"/>
+      <c r="H52" s="14"/>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A53" s="17"/>
-      <c r="B53" s="17"/>
-      <c r="C53" s="17"/>
-      <c r="D53" s="17"/>
-      <c r="E53" s="17"/>
-      <c r="F53" s="17"/>
-      <c r="H53" s="17"/>
+      <c r="A53" s="14"/>
+      <c r="B53" s="14"/>
+      <c r="C53" s="14"/>
+      <c r="D53" s="14"/>
+      <c r="E53" s="14"/>
+      <c r="F53" s="14"/>
+      <c r="H53" s="14"/>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A54" s="17"/>
-      <c r="B54" s="17"/>
-      <c r="C54" s="17"/>
-      <c r="D54" s="17"/>
-      <c r="E54" s="17"/>
-      <c r="F54" s="17"/>
-      <c r="H54" s="17"/>
+      <c r="A54" s="14"/>
+      <c r="B54" s="14"/>
+      <c r="C54" s="14"/>
+      <c r="D54" s="14"/>
+      <c r="E54" s="14"/>
+      <c r="F54" s="14"/>
+      <c r="H54" s="14"/>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A55" s="17"/>
-      <c r="B55" s="17"/>
-      <c r="C55" s="17"/>
-      <c r="D55" s="17"/>
-      <c r="E55" s="17"/>
-      <c r="F55" s="17"/>
-      <c r="H55" s="17"/>
+      <c r="A55" s="14"/>
+      <c r="B55" s="14"/>
+      <c r="C55" s="14"/>
+      <c r="D55" s="14"/>
+      <c r="E55" s="14"/>
+      <c r="F55" s="14"/>
+      <c r="H55" s="14"/>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A56" s="17"/>
-      <c r="B56" s="17"/>
-      <c r="C56" s="17"/>
-      <c r="D56" s="17"/>
-      <c r="E56" s="17"/>
-      <c r="F56" s="17"/>
-      <c r="H56" s="17"/>
+      <c r="A56" s="14"/>
+      <c r="B56" s="14"/>
+      <c r="C56" s="14"/>
+      <c r="D56" s="14"/>
+      <c r="E56" s="14"/>
+      <c r="F56" s="14"/>
+      <c r="H56" s="14"/>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A57" s="17"/>
-      <c r="B57" s="17"/>
-      <c r="C57" s="17"/>
-      <c r="D57" s="17"/>
-      <c r="E57" s="17"/>
-      <c r="F57" s="17"/>
-      <c r="H57" s="17"/>
+      <c r="A57" s="14"/>
+      <c r="B57" s="14"/>
+      <c r="C57" s="14"/>
+      <c r="D57" s="14"/>
+      <c r="E57" s="14"/>
+      <c r="F57" s="14"/>
+      <c r="H57" s="14"/>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A58" s="17"/>
-      <c r="B58" s="17"/>
-      <c r="C58" s="17"/>
-      <c r="D58" s="17"/>
-      <c r="E58" s="17"/>
-      <c r="F58" s="17"/>
-      <c r="H58" s="17"/>
+      <c r="A58" s="14"/>
+      <c r="B58" s="14"/>
+      <c r="C58" s="14"/>
+      <c r="D58" s="14"/>
+      <c r="E58" s="14"/>
+      <c r="F58" s="14"/>
+      <c r="H58" s="14"/>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A59" s="17"/>
-      <c r="B59" s="17"/>
-      <c r="C59" s="17"/>
-      <c r="D59" s="17"/>
-      <c r="E59" s="17"/>
-      <c r="F59" s="17"/>
-      <c r="H59" s="17"/>
+      <c r="A59" s="14"/>
+      <c r="B59" s="14"/>
+      <c r="C59" s="14"/>
+      <c r="D59" s="14"/>
+      <c r="E59" s="14"/>
+      <c r="F59" s="14"/>
+      <c r="H59" s="14"/>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A60" s="17"/>
-      <c r="B60" s="17"/>
-      <c r="C60" s="17"/>
-      <c r="D60" s="17"/>
-      <c r="E60" s="17"/>
-      <c r="F60" s="17"/>
-      <c r="H60" s="17"/>
+      <c r="A60" s="14"/>
+      <c r="B60" s="14"/>
+      <c r="C60" s="14"/>
+      <c r="D60" s="14"/>
+      <c r="E60" s="14"/>
+      <c r="F60" s="14"/>
+      <c r="H60" s="14"/>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A61" s="17"/>
-      <c r="B61" s="17"/>
-      <c r="C61" s="17"/>
-      <c r="D61" s="17"/>
-      <c r="E61" s="17"/>
-      <c r="F61" s="17"/>
-      <c r="H61" s="17"/>
+      <c r="A61" s="14"/>
+      <c r="B61" s="14"/>
+      <c r="C61" s="14"/>
+      <c r="D61" s="14"/>
+      <c r="E61" s="14"/>
+      <c r="F61" s="14"/>
+      <c r="H61" s="14"/>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A62" s="17"/>
-      <c r="B62" s="17"/>
-      <c r="C62" s="17"/>
-      <c r="D62" s="17"/>
-      <c r="E62" s="17"/>
-      <c r="F62" s="17"/>
-      <c r="H62" s="17"/>
+      <c r="A62" s="14"/>
+      <c r="B62" s="14"/>
+      <c r="C62" s="14"/>
+      <c r="D62" s="14"/>
+      <c r="E62" s="14"/>
+      <c r="F62" s="14"/>
+      <c r="H62" s="14"/>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A63" s="17"/>
-      <c r="B63" s="17"/>
-      <c r="C63" s="17"/>
-      <c r="D63" s="17"/>
-      <c r="E63" s="17"/>
-      <c r="F63" s="17"/>
-      <c r="H63" s="17"/>
+      <c r="A63" s="14"/>
+      <c r="B63" s="14"/>
+      <c r="C63" s="14"/>
+      <c r="D63" s="14"/>
+      <c r="E63" s="14"/>
+      <c r="F63" s="14"/>
+      <c r="H63" s="14"/>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A64" s="17"/>
-      <c r="B64" s="17"/>
-      <c r="C64" s="17"/>
-      <c r="D64" s="17"/>
-      <c r="E64" s="17"/>
-      <c r="F64" s="17"/>
-      <c r="H64" s="17"/>
+      <c r="A64" s="14"/>
+      <c r="B64" s="14"/>
+      <c r="C64" s="14"/>
+      <c r="D64" s="14"/>
+      <c r="E64" s="14"/>
+      <c r="F64" s="14"/>
+      <c r="H64" s="14"/>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A65" s="17"/>
-      <c r="B65" s="17"/>
-      <c r="C65" s="17"/>
-      <c r="D65" s="17"/>
-      <c r="E65" s="17"/>
-      <c r="F65" s="17"/>
-      <c r="H65" s="17"/>
+      <c r="A65" s="14"/>
+      <c r="B65" s="14"/>
+      <c r="C65" s="14"/>
+      <c r="D65" s="14"/>
+      <c r="E65" s="14"/>
+      <c r="F65" s="14"/>
+      <c r="H65" s="14"/>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A66" s="17"/>
-      <c r="B66" s="17"/>
-      <c r="C66" s="17"/>
-      <c r="D66" s="17"/>
-      <c r="E66" s="17"/>
-      <c r="F66" s="17"/>
-      <c r="H66" s="17"/>
+      <c r="A66" s="14"/>
+      <c r="B66" s="14"/>
+      <c r="C66" s="14"/>
+      <c r="D66" s="14"/>
+      <c r="E66" s="14"/>
+      <c r="F66" s="14"/>
+      <c r="H66" s="14"/>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A67" s="17"/>
-      <c r="B67" s="17"/>
-      <c r="C67" s="17"/>
-      <c r="D67" s="17"/>
-      <c r="E67" s="17"/>
-      <c r="F67" s="17"/>
-      <c r="H67" s="17"/>
+      <c r="A67" s="14"/>
+      <c r="B67" s="14"/>
+      <c r="C67" s="14"/>
+      <c r="D67" s="14"/>
+      <c r="E67" s="14"/>
+      <c r="F67" s="14"/>
+      <c r="H67" s="14"/>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A68" s="17"/>
-      <c r="B68" s="17"/>
-      <c r="C68" s="17"/>
-      <c r="D68" s="17"/>
-      <c r="E68" s="17"/>
-      <c r="F68" s="17"/>
-      <c r="H68" s="17"/>
+      <c r="A68" s="14"/>
+      <c r="B68" s="14"/>
+      <c r="C68" s="14"/>
+      <c r="D68" s="14"/>
+      <c r="E68" s="14"/>
+      <c r="F68" s="14"/>
+      <c r="H68" s="14"/>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A69" s="17"/>
-      <c r="B69" s="17"/>
-      <c r="C69" s="17"/>
-      <c r="D69" s="17"/>
-      <c r="E69" s="17"/>
-      <c r="F69" s="17"/>
-      <c r="H69" s="17"/>
+      <c r="A69" s="14"/>
+      <c r="B69" s="14"/>
+      <c r="C69" s="14"/>
+      <c r="D69" s="14"/>
+      <c r="E69" s="14"/>
+      <c r="F69" s="14"/>
+      <c r="H69" s="14"/>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A70" s="17"/>
-      <c r="B70" s="17"/>
-      <c r="C70" s="17"/>
-      <c r="D70" s="17"/>
-      <c r="E70" s="17"/>
-      <c r="F70" s="17"/>
-      <c r="H70" s="17"/>
+      <c r="A70" s="14"/>
+      <c r="B70" s="14"/>
+      <c r="C70" s="14"/>
+      <c r="D70" s="14"/>
+      <c r="E70" s="14"/>
+      <c r="F70" s="14"/>
+      <c r="H70" s="14"/>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A71" s="17"/>
-      <c r="B71" s="17"/>
-      <c r="C71" s="17"/>
-      <c r="D71" s="17"/>
-      <c r="E71" s="17"/>
-      <c r="F71" s="17"/>
-      <c r="H71" s="17"/>
+      <c r="A71" s="14"/>
+      <c r="B71" s="14"/>
+      <c r="C71" s="14"/>
+      <c r="D71" s="14"/>
+      <c r="E71" s="14"/>
+      <c r="F71" s="14"/>
+      <c r="H71" s="14"/>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A72" s="17"/>
-      <c r="B72" s="17"/>
-      <c r="C72" s="17"/>
-      <c r="D72" s="17"/>
-      <c r="E72" s="17"/>
-      <c r="F72" s="17"/>
-      <c r="H72" s="17"/>
+      <c r="A72" s="14"/>
+      <c r="B72" s="14"/>
+      <c r="C72" s="14"/>
+      <c r="D72" s="14"/>
+      <c r="E72" s="14"/>
+      <c r="F72" s="14"/>
+      <c r="H72" s="14"/>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A73" s="17"/>
-      <c r="B73" s="17"/>
-      <c r="C73" s="17"/>
-      <c r="D73" s="17"/>
-      <c r="E73" s="17"/>
-      <c r="F73" s="17"/>
-      <c r="H73" s="17"/>
+      <c r="A73" s="14"/>
+      <c r="B73" s="14"/>
+      <c r="C73" s="14"/>
+      <c r="D73" s="14"/>
+      <c r="E73" s="14"/>
+      <c r="F73" s="14"/>
+      <c r="H73" s="14"/>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A74" s="17"/>
-      <c r="B74" s="17"/>
-      <c r="C74" s="17"/>
-      <c r="D74" s="17"/>
-      <c r="E74" s="17"/>
-      <c r="F74" s="17"/>
-      <c r="H74" s="17"/>
+      <c r="A74" s="14"/>
+      <c r="B74" s="14"/>
+      <c r="C74" s="14"/>
+      <c r="D74" s="14"/>
+      <c r="E74" s="14"/>
+      <c r="F74" s="14"/>
+      <c r="H74" s="14"/>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A75" s="17"/>
-      <c r="B75" s="17"/>
-      <c r="C75" s="17"/>
-      <c r="D75" s="17"/>
-      <c r="E75" s="17"/>
-      <c r="F75" s="17"/>
-      <c r="H75" s="17"/>
+      <c r="A75" s="14"/>
+      <c r="B75" s="14"/>
+      <c r="C75" s="14"/>
+      <c r="D75" s="14"/>
+      <c r="E75" s="14"/>
+      <c r="F75" s="14"/>
+      <c r="H75" s="14"/>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A76" s="17"/>
-      <c r="B76" s="17"/>
-      <c r="C76" s="17"/>
-      <c r="D76" s="17"/>
-      <c r="E76" s="17"/>
-      <c r="F76" s="17"/>
-      <c r="H76" s="17"/>
+      <c r="A76" s="14"/>
+      <c r="B76" s="14"/>
+      <c r="C76" s="14"/>
+      <c r="D76" s="14"/>
+      <c r="E76" s="14"/>
+      <c r="F76" s="14"/>
+      <c r="H76" s="14"/>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A77" s="17"/>
-      <c r="B77" s="17"/>
-      <c r="C77" s="17"/>
-      <c r="D77" s="17"/>
-      <c r="E77" s="17"/>
-      <c r="F77" s="17"/>
-      <c r="H77" s="17"/>
+      <c r="A77" s="14"/>
+      <c r="B77" s="14"/>
+      <c r="C77" s="14"/>
+      <c r="D77" s="14"/>
+      <c r="E77" s="14"/>
+      <c r="F77" s="14"/>
+      <c r="H77" s="14"/>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A78" s="17"/>
-      <c r="B78" s="17"/>
-      <c r="C78" s="17"/>
-      <c r="D78" s="17"/>
-      <c r="E78" s="17"/>
-      <c r="F78" s="17"/>
-      <c r="H78" s="17"/>
+      <c r="A78" s="14"/>
+      <c r="B78" s="14"/>
+      <c r="C78" s="14"/>
+      <c r="D78" s="14"/>
+      <c r="E78" s="14"/>
+      <c r="F78" s="14"/>
+      <c r="H78" s="14"/>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A79" s="17"/>
-      <c r="B79" s="17"/>
-      <c r="C79" s="17"/>
-      <c r="D79" s="17"/>
-      <c r="E79" s="17"/>
-      <c r="F79" s="17"/>
-      <c r="H79" s="17"/>
+      <c r="A79" s="14"/>
+      <c r="B79" s="14"/>
+      <c r="C79" s="14"/>
+      <c r="D79" s="14"/>
+      <c r="E79" s="14"/>
+      <c r="F79" s="14"/>
+      <c r="H79" s="14"/>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A80" s="17"/>
-      <c r="B80" s="17"/>
-      <c r="C80" s="17"/>
-      <c r="D80" s="17"/>
-      <c r="E80" s="17"/>
-      <c r="F80" s="17"/>
-      <c r="H80" s="17"/>
+      <c r="A80" s="14"/>
+      <c r="B80" s="14"/>
+      <c r="C80" s="14"/>
+      <c r="D80" s="14"/>
+      <c r="E80" s="14"/>
+      <c r="F80" s="14"/>
+      <c r="H80" s="14"/>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A81" s="17"/>
-      <c r="B81" s="17"/>
-      <c r="C81" s="17"/>
-      <c r="D81" s="17"/>
-      <c r="E81" s="17"/>
-      <c r="F81" s="17"/>
-      <c r="H81" s="17"/>
+      <c r="A81" s="14"/>
+      <c r="B81" s="14"/>
+      <c r="C81" s="14"/>
+      <c r="D81" s="14"/>
+      <c r="E81" s="14"/>
+      <c r="F81" s="14"/>
+      <c r="H81" s="14"/>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A82" s="17"/>
-      <c r="B82" s="17"/>
-      <c r="C82" s="17"/>
-      <c r="D82" s="17"/>
-      <c r="E82" s="17"/>
-      <c r="F82" s="17"/>
-      <c r="H82" s="17"/>
+      <c r="A82" s="14"/>
+      <c r="B82" s="14"/>
+      <c r="C82" s="14"/>
+      <c r="D82" s="14"/>
+      <c r="E82" s="14"/>
+      <c r="F82" s="14"/>
+      <c r="H82" s="14"/>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A83" s="17"/>
-      <c r="B83" s="17"/>
-      <c r="C83" s="17"/>
-      <c r="D83" s="17"/>
-      <c r="E83" s="17"/>
-      <c r="F83" s="17"/>
-      <c r="H83" s="17"/>
+      <c r="A83" s="14"/>
+      <c r="B83" s="14"/>
+      <c r="C83" s="14"/>
+      <c r="D83" s="14"/>
+      <c r="E83" s="14"/>
+      <c r="F83" s="14"/>
+      <c r="H83" s="14"/>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A84" s="17"/>
-      <c r="B84" s="17"/>
-      <c r="C84" s="17"/>
-      <c r="D84" s="17"/>
-      <c r="E84" s="17"/>
-      <c r="F84" s="17"/>
-      <c r="H84" s="17"/>
+      <c r="A84" s="14"/>
+      <c r="B84" s="14"/>
+      <c r="C84" s="14"/>
+      <c r="D84" s="14"/>
+      <c r="E84" s="14"/>
+      <c r="F84" s="14"/>
+      <c r="H84" s="14"/>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A85" s="17"/>
-      <c r="B85" s="17"/>
-      <c r="C85" s="17"/>
-      <c r="D85" s="17"/>
-      <c r="E85" s="17"/>
-      <c r="F85" s="17"/>
-      <c r="H85" s="17"/>
+      <c r="A85" s="14"/>
+      <c r="B85" s="14"/>
+      <c r="C85" s="14"/>
+      <c r="D85" s="14"/>
+      <c r="E85" s="14"/>
+      <c r="F85" s="14"/>
+      <c r="H85" s="14"/>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A86" s="17"/>
-      <c r="B86" s="17"/>
-      <c r="C86" s="17"/>
-      <c r="D86" s="17"/>
-      <c r="E86" s="17"/>
-      <c r="F86" s="17"/>
-      <c r="H86" s="17"/>
+      <c r="A86" s="14"/>
+      <c r="B86" s="14"/>
+      <c r="C86" s="14"/>
+      <c r="D86" s="14"/>
+      <c r="E86" s="14"/>
+      <c r="F86" s="14"/>
+      <c r="H86" s="14"/>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A87" s="17"/>
-      <c r="B87" s="17"/>
-      <c r="C87" s="17"/>
-      <c r="D87" s="17"/>
-      <c r="E87" s="17"/>
-      <c r="F87" s="17"/>
-      <c r="H87" s="17"/>
+      <c r="A87" s="14"/>
+      <c r="B87" s="14"/>
+      <c r="C87" s="14"/>
+      <c r="D87" s="14"/>
+      <c r="E87" s="14"/>
+      <c r="F87" s="14"/>
+      <c r="H87" s="14"/>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A88" s="17"/>
-      <c r="B88" s="17"/>
-      <c r="C88" s="17"/>
-      <c r="D88" s="17"/>
-      <c r="E88" s="17"/>
-      <c r="F88" s="17"/>
-      <c r="H88" s="17"/>
+      <c r="A88" s="14"/>
+      <c r="B88" s="14"/>
+      <c r="C88" s="14"/>
+      <c r="D88" s="14"/>
+      <c r="E88" s="14"/>
+      <c r="F88" s="14"/>
+      <c r="H88" s="14"/>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A89" s="17"/>
-      <c r="B89" s="17"/>
-      <c r="C89" s="17"/>
-      <c r="D89" s="17"/>
-      <c r="E89" s="17"/>
-      <c r="F89" s="17"/>
-      <c r="H89" s="17"/>
+      <c r="A89" s="14"/>
+      <c r="B89" s="14"/>
+      <c r="C89" s="14"/>
+      <c r="D89" s="14"/>
+      <c r="E89" s="14"/>
+      <c r="F89" s="14"/>
+      <c r="H89" s="14"/>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A90" s="17"/>
-      <c r="B90" s="17"/>
-      <c r="C90" s="17"/>
-      <c r="D90" s="17"/>
-      <c r="E90" s="17"/>
-      <c r="F90" s="17"/>
-      <c r="H90" s="17"/>
+      <c r="A90" s="14"/>
+      <c r="B90" s="14"/>
+      <c r="C90" s="14"/>
+      <c r="D90" s="14"/>
+      <c r="E90" s="14"/>
+      <c r="F90" s="14"/>
+      <c r="H90" s="14"/>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A91" s="17"/>
-      <c r="B91" s="17"/>
-      <c r="C91" s="17"/>
-      <c r="D91" s="17"/>
-      <c r="E91" s="17"/>
-      <c r="F91" s="17"/>
-      <c r="H91" s="17"/>
+      <c r="A91" s="14"/>
+      <c r="B91" s="14"/>
+      <c r="C91" s="14"/>
+      <c r="D91" s="14"/>
+      <c r="E91" s="14"/>
+      <c r="F91" s="14"/>
+      <c r="H91" s="14"/>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A92" s="17"/>
-      <c r="B92" s="17"/>
-      <c r="C92" s="17"/>
-      <c r="D92" s="17"/>
-      <c r="E92" s="17"/>
-      <c r="F92" s="17"/>
-      <c r="H92" s="17"/>
+      <c r="A92" s="14"/>
+      <c r="B92" s="14"/>
+      <c r="C92" s="14"/>
+      <c r="D92" s="14"/>
+      <c r="E92" s="14"/>
+      <c r="F92" s="14"/>
+      <c r="H92" s="14"/>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A93" s="17"/>
-      <c r="B93" s="17"/>
-      <c r="C93" s="17"/>
-      <c r="D93" s="17"/>
-      <c r="E93" s="17"/>
-      <c r="F93" s="17"/>
-      <c r="H93" s="17"/>
+      <c r="A93" s="14"/>
+      <c r="B93" s="14"/>
+      <c r="C93" s="14"/>
+      <c r="D93" s="14"/>
+      <c r="E93" s="14"/>
+      <c r="F93" s="14"/>
+      <c r="H93" s="14"/>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A94" s="17"/>
-      <c r="B94" s="17"/>
-      <c r="C94" s="17"/>
-      <c r="D94" s="17"/>
-      <c r="E94" s="17"/>
-      <c r="F94" s="17"/>
-      <c r="H94" s="17"/>
+      <c r="A94" s="14"/>
+      <c r="B94" s="14"/>
+      <c r="C94" s="14"/>
+      <c r="D94" s="14"/>
+      <c r="E94" s="14"/>
+      <c r="F94" s="14"/>
+      <c r="H94" s="14"/>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A95" s="17"/>
-      <c r="B95" s="17"/>
-      <c r="C95" s="17"/>
-      <c r="D95" s="17"/>
-      <c r="E95" s="17"/>
-      <c r="F95" s="17"/>
-      <c r="H95" s="17"/>
+      <c r="A95" s="14"/>
+      <c r="B95" s="14"/>
+      <c r="C95" s="14"/>
+      <c r="D95" s="14"/>
+      <c r="E95" s="14"/>
+      <c r="F95" s="14"/>
+      <c r="H95" s="14"/>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A96" s="17"/>
-      <c r="B96" s="17"/>
-      <c r="C96" s="17"/>
-      <c r="D96" s="17"/>
-      <c r="E96" s="17"/>
-      <c r="F96" s="17"/>
-      <c r="H96" s="17"/>
+      <c r="A96" s="14"/>
+      <c r="B96" s="14"/>
+      <c r="C96" s="14"/>
+      <c r="D96" s="14"/>
+      <c r="E96" s="14"/>
+      <c r="F96" s="14"/>
+      <c r="H96" s="14"/>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A97" s="17"/>
-      <c r="B97" s="17"/>
-      <c r="C97" s="17"/>
-      <c r="D97" s="17"/>
-      <c r="E97" s="17"/>
-      <c r="F97" s="17"/>
-      <c r="H97" s="17"/>
+      <c r="A97" s="14"/>
+      <c r="B97" s="14"/>
+      <c r="C97" s="14"/>
+      <c r="D97" s="14"/>
+      <c r="E97" s="14"/>
+      <c r="F97" s="14"/>
+      <c r="H97" s="14"/>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A98" s="17"/>
-      <c r="B98" s="17"/>
-      <c r="C98" s="17"/>
-      <c r="D98" s="17"/>
-      <c r="E98" s="17"/>
-      <c r="F98" s="17"/>
-      <c r="H98" s="17"/>
+      <c r="A98" s="14"/>
+      <c r="B98" s="14"/>
+      <c r="C98" s="14"/>
+      <c r="D98" s="14"/>
+      <c r="E98" s="14"/>
+      <c r="F98" s="14"/>
+      <c r="H98" s="14"/>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A99" s="17"/>
-      <c r="B99" s="17"/>
-      <c r="C99" s="17"/>
-      <c r="D99" s="17"/>
-      <c r="E99" s="17"/>
-      <c r="F99" s="17"/>
-      <c r="H99" s="17"/>
+      <c r="A99" s="14"/>
+      <c r="B99" s="14"/>
+      <c r="C99" s="14"/>
+      <c r="D99" s="14"/>
+      <c r="E99" s="14"/>
+      <c r="F99" s="14"/>
+      <c r="H99" s="14"/>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A100" s="17"/>
-      <c r="B100" s="17"/>
-      <c r="C100" s="17"/>
-      <c r="D100" s="17"/>
-      <c r="E100" s="17"/>
-      <c r="F100" s="17"/>
-      <c r="H100" s="17"/>
+      <c r="A100" s="14"/>
+      <c r="B100" s="14"/>
+      <c r="C100" s="14"/>
+      <c r="D100" s="14"/>
+      <c r="E100" s="14"/>
+      <c r="F100" s="14"/>
+      <c r="H100" s="14"/>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A101" s="17"/>
-      <c r="B101" s="17"/>
-      <c r="C101" s="17"/>
-      <c r="D101" s="17"/>
-      <c r="E101" s="17"/>
-      <c r="F101" s="17"/>
-      <c r="H101" s="17"/>
+      <c r="A101" s="14"/>
+      <c r="B101" s="14"/>
+      <c r="C101" s="14"/>
+      <c r="D101" s="14"/>
+      <c r="E101" s="14"/>
+      <c r="F101" s="14"/>
+      <c r="H101" s="14"/>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A102" s="17"/>
-      <c r="B102" s="17"/>
-      <c r="C102" s="17"/>
-      <c r="D102" s="17"/>
-      <c r="E102" s="17"/>
-      <c r="F102" s="17"/>
-      <c r="H102" s="17"/>
+      <c r="A102" s="14"/>
+      <c r="B102" s="14"/>
+      <c r="C102" s="14"/>
+      <c r="D102" s="14"/>
+      <c r="E102" s="14"/>
+      <c r="F102" s="14"/>
+      <c r="H102" s="14"/>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A103" s="17"/>
-      <c r="B103" s="17"/>
-      <c r="C103" s="17"/>
-      <c r="D103" s="17"/>
-      <c r="E103" s="17"/>
-      <c r="F103" s="17"/>
-      <c r="H103" s="17"/>
+      <c r="A103" s="14"/>
+      <c r="B103" s="14"/>
+      <c r="C103" s="14"/>
+      <c r="D103" s="14"/>
+      <c r="E103" s="14"/>
+      <c r="F103" s="14"/>
+      <c r="H103" s="14"/>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A104" s="17"/>
-      <c r="B104" s="17"/>
-      <c r="C104" s="17"/>
-      <c r="D104" s="17"/>
-      <c r="E104" s="17"/>
-      <c r="F104" s="17"/>
-      <c r="H104" s="17"/>
+      <c r="A104" s="14"/>
+      <c r="B104" s="14"/>
+      <c r="C104" s="14"/>
+      <c r="D104" s="14"/>
+      <c r="E104" s="14"/>
+      <c r="F104" s="14"/>
+      <c r="H104" s="14"/>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A105" s="17"/>
-      <c r="B105" s="17"/>
-      <c r="C105" s="17"/>
-      <c r="D105" s="17"/>
-      <c r="E105" s="17"/>
-      <c r="F105" s="17"/>
-      <c r="H105" s="17"/>
+      <c r="A105" s="14"/>
+      <c r="B105" s="14"/>
+      <c r="C105" s="14"/>
+      <c r="D105" s="14"/>
+      <c r="E105" s="14"/>
+      <c r="F105" s="14"/>
+      <c r="H105" s="14"/>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A106" s="17"/>
-      <c r="B106" s="17"/>
-      <c r="C106" s="17"/>
-      <c r="D106" s="17"/>
-      <c r="E106" s="17"/>
-      <c r="F106" s="17"/>
-      <c r="H106" s="17"/>
-    </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A107" s="17"/>
-      <c r="B107" s="17"/>
-      <c r="C107" s="17"/>
-      <c r="D107" s="17"/>
-      <c r="E107" s="17"/>
-      <c r="F107" s="17"/>
-      <c r="H107" s="17"/>
-    </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A108" s="17"/>
-      <c r="B108" s="17"/>
-      <c r="C108" s="17"/>
-      <c r="D108" s="17"/>
-      <c r="E108" s="17"/>
-      <c r="F108" s="17"/>
-      <c r="H108" s="17"/>
-    </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A109" s="17"/>
-      <c r="B109" s="17"/>
-      <c r="C109" s="17"/>
-      <c r="D109" s="17"/>
-      <c r="E109" s="17"/>
-      <c r="F109" s="17"/>
-      <c r="H109" s="17"/>
-    </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A110" s="17"/>
-      <c r="B110" s="17"/>
-      <c r="C110" s="17"/>
-      <c r="D110" s="17"/>
-      <c r="E110" s="17"/>
-      <c r="F110" s="17"/>
-      <c r="H110" s="17"/>
-    </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A111" s="17"/>
-      <c r="B111" s="17"/>
-      <c r="C111" s="17"/>
-      <c r="D111" s="17"/>
-      <c r="E111" s="17"/>
-      <c r="F111" s="17"/>
-      <c r="H111" s="17"/>
-    </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A112" s="17"/>
-      <c r="B112" s="17"/>
-      <c r="C112" s="17"/>
-      <c r="D112" s="17"/>
-      <c r="E112" s="17"/>
-      <c r="F112" s="17"/>
-      <c r="H112" s="17"/>
-    </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A113" s="17"/>
-      <c r="B113" s="17"/>
-      <c r="C113" s="17"/>
-      <c r="D113" s="17"/>
-      <c r="E113" s="17"/>
-      <c r="F113" s="17"/>
-      <c r="H113" s="17"/>
-    </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A114" s="17"/>
-      <c r="B114" s="17"/>
-      <c r="C114" s="17"/>
-      <c r="D114" s="17"/>
-      <c r="E114" s="17"/>
-      <c r="F114" s="17"/>
-      <c r="H114" s="17"/>
-    </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A115" s="17"/>
-      <c r="B115" s="17"/>
-      <c r="C115" s="17"/>
-      <c r="D115" s="17"/>
-      <c r="E115" s="17"/>
-      <c r="F115" s="17"/>
-      <c r="H115" s="17"/>
-    </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A116" s="17"/>
-      <c r="B116" s="17"/>
-      <c r="C116" s="17"/>
-      <c r="D116" s="17"/>
-      <c r="E116" s="17"/>
-      <c r="F116" s="17"/>
-      <c r="H116" s="17"/>
-    </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A117" s="17"/>
-      <c r="B117" s="17"/>
-      <c r="C117" s="17"/>
-      <c r="D117" s="17"/>
-      <c r="E117" s="17"/>
-      <c r="F117" s="17"/>
-      <c r="H117" s="17"/>
-    </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A118" s="17"/>
-      <c r="B118" s="17"/>
-      <c r="C118" s="17"/>
-      <c r="D118" s="17"/>
-      <c r="E118" s="17"/>
-      <c r="F118" s="17"/>
-      <c r="H118" s="17"/>
-    </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A119" s="17"/>
-      <c r="B119" s="17"/>
-      <c r="C119" s="17"/>
-      <c r="D119" s="17"/>
-      <c r="E119" s="17"/>
-      <c r="F119" s="17"/>
-      <c r="H119" s="17"/>
-    </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A120" s="17"/>
-      <c r="B120" s="17"/>
-      <c r="C120" s="17"/>
-      <c r="D120" s="17"/>
-      <c r="E120" s="17"/>
-      <c r="F120" s="17"/>
-      <c r="H120" s="17"/>
-    </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A121" s="17"/>
-      <c r="B121" s="17"/>
-      <c r="C121" s="17"/>
-      <c r="D121" s="17"/>
-      <c r="E121" s="17"/>
-      <c r="F121" s="17"/>
-      <c r="H121" s="17"/>
-    </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A122" s="17"/>
-      <c r="B122" s="17"/>
-      <c r="C122" s="17"/>
-      <c r="D122" s="17"/>
-      <c r="E122" s="17"/>
-      <c r="F122" s="17"/>
-      <c r="H122" s="17"/>
-    </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A123" s="17"/>
-      <c r="B123" s="17"/>
-      <c r="C123" s="17"/>
-      <c r="D123" s="17"/>
-      <c r="E123" s="17"/>
-      <c r="F123" s="17"/>
-      <c r="H123" s="17"/>
+      <c r="A106" s="14"/>
+      <c r="B106" s="14"/>
+      <c r="C106" s="14"/>
+      <c r="D106" s="14"/>
+      <c r="E106" s="14"/>
+      <c r="F106" s="14"/>
+      <c r="H106" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2860,10 +2823,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E7E83A2-0C01-4873-A759-2E5A62E8D39F}">
-  <dimension ref="A1:E124"/>
+  <dimension ref="A1:E127"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="D5" sqref="D2:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2880,25 +2843,25 @@
         <v>124</v>
       </c>
       <c r="B1" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="D1" t="s">
         <v>124</v>
       </c>
       <c r="E1" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>125</v>
+        <v>196</v>
       </c>
       <c r="B2" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
         <v>OK</v>
       </c>
       <c r="D2" t="s">
-        <v>155</v>
+        <v>212</v>
       </c>
       <c r="E2" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -2907,62 +2870,62 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>126</v>
+        <v>197</v>
       </c>
       <c r="B3" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
         <v>OK</v>
       </c>
       <c r="D3" t="s">
-        <v>156</v>
+        <v>213</v>
       </c>
       <c r="E3" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
-        <v>OK</v>
+        <v>FALTA</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>127</v>
+        <v>198</v>
       </c>
       <c r="B4" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
-        <v>OK</v>
+        <v>FALTA</v>
       </c>
       <c r="D4" t="s">
-        <v>157</v>
+        <v>214</v>
       </c>
       <c r="E4" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
-        <v>OK</v>
+        <v>FALTA</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>128</v>
+        <v>199</v>
       </c>
       <c r="B5" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
-        <v>OK</v>
+        <v>FALTA</v>
       </c>
       <c r="D5" t="s">
-        <v>158</v>
+        <v>215</v>
       </c>
       <c r="E5" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
-        <v>OK</v>
+        <v>FALTA</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>129</v>
+        <v>200</v>
       </c>
       <c r="B6" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
         <v>OK</v>
       </c>
       <c r="D6" t="s">
-        <v>159</v>
+        <v>41</v>
       </c>
       <c r="E6" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -2971,14 +2934,14 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>130</v>
+        <v>201</v>
       </c>
       <c r="B7" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
         <v>OK</v>
       </c>
       <c r="D7" t="s">
-        <v>160</v>
+        <v>149</v>
       </c>
       <c r="E7" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -2987,14 +2950,14 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>131</v>
+        <v>202</v>
       </c>
       <c r="B8" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
         <v>OK</v>
       </c>
       <c r="D8" t="s">
-        <v>161</v>
+        <v>42</v>
       </c>
       <c r="E8" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3003,14 +2966,14 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>132</v>
+        <v>203</v>
       </c>
       <c r="B9" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
         <v>OK</v>
       </c>
       <c r="D9" t="s">
-        <v>162</v>
+        <v>150</v>
       </c>
       <c r="E9" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3019,14 +2982,14 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>133</v>
+        <v>204</v>
       </c>
       <c r="B10" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
         <v>OK</v>
       </c>
       <c r="D10" t="s">
-        <v>163</v>
+        <v>43</v>
       </c>
       <c r="E10" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3035,14 +2998,14 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>134</v>
+        <v>205</v>
       </c>
       <c r="B11" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
         <v>OK</v>
       </c>
       <c r="D11" t="s">
-        <v>164</v>
+        <v>151</v>
       </c>
       <c r="E11" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3051,14 +3014,14 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>135</v>
+        <v>206</v>
       </c>
       <c r="B12" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
-        <v>OK</v>
+        <v>FALTA</v>
       </c>
       <c r="D12" t="s">
-        <v>165</v>
+        <v>44</v>
       </c>
       <c r="E12" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3067,14 +3030,14 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>136</v>
+        <v>207</v>
       </c>
       <c r="B13" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
         <v>OK</v>
       </c>
       <c r="D13" t="s">
-        <v>166</v>
+        <v>45</v>
       </c>
       <c r="E13" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3083,14 +3046,14 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>137</v>
+        <v>208</v>
       </c>
       <c r="B14" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
         <v>OK</v>
       </c>
       <c r="D14" t="s">
-        <v>167</v>
+        <v>46</v>
       </c>
       <c r="E14" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3099,14 +3062,14 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>138</v>
+        <v>209</v>
       </c>
       <c r="B15" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
         <v>OK</v>
       </c>
       <c r="D15" t="s">
-        <v>168</v>
+        <v>152</v>
       </c>
       <c r="E15" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3115,14 +3078,14 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>140</v>
-      </c>
-      <c r="B16" t="str">
+        <v>210</v>
+      </c>
+      <c r="B16" s="16" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
         <v>OK</v>
       </c>
       <c r="D16" t="s">
-        <v>169</v>
+        <v>153</v>
       </c>
       <c r="E16" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3131,14 +3094,14 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>139</v>
-      </c>
-      <c r="B17" t="str">
-        <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
-        <v>OK</v>
+        <v>211</v>
+      </c>
+      <c r="B17" s="16" t="str">
+        <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
+        <v>FALTA</v>
       </c>
       <c r="D17" t="s">
-        <v>170</v>
+        <v>47</v>
       </c>
       <c r="E17" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3147,14 +3110,14 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>141</v>
+        <v>0</v>
       </c>
       <c r="B18" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
         <v>OK</v>
       </c>
       <c r="D18" t="s">
-        <v>171</v>
+        <v>154</v>
       </c>
       <c r="E18" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3163,14 +3126,14 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>142</v>
+        <v>1</v>
       </c>
       <c r="B19" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
         <v>OK</v>
       </c>
       <c r="D19" t="s">
-        <v>172</v>
+        <v>48</v>
       </c>
       <c r="E19" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3179,14 +3142,14 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>143</v>
+        <v>2</v>
       </c>
       <c r="B20" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
         <v>OK</v>
       </c>
       <c r="D20" t="s">
-        <v>173</v>
+        <v>49</v>
       </c>
       <c r="E20" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3195,14 +3158,14 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>146</v>
+        <v>3</v>
       </c>
       <c r="B21" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
         <v>OK</v>
       </c>
       <c r="D21" t="s">
-        <v>174</v>
+        <v>50</v>
       </c>
       <c r="E21" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3211,14 +3174,14 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>144</v>
+        <v>4</v>
       </c>
       <c r="B22" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
         <v>OK</v>
       </c>
       <c r="D22" t="s">
-        <v>175</v>
+        <v>155</v>
       </c>
       <c r="E22" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3227,14 +3190,14 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>145</v>
+        <v>125</v>
       </c>
       <c r="B23" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
         <v>OK</v>
       </c>
       <c r="D23" t="s">
-        <v>176</v>
+        <v>156</v>
       </c>
       <c r="E23" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3243,14 +3206,14 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>147</v>
+        <v>126</v>
       </c>
       <c r="B24" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
         <v>OK</v>
       </c>
       <c r="D24" t="s">
-        <v>177</v>
+        <v>51</v>
       </c>
       <c r="E24" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3259,14 +3222,14 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>148</v>
+        <v>5</v>
       </c>
       <c r="B25" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
         <v>OK</v>
       </c>
       <c r="D25" t="s">
-        <v>178</v>
+        <v>52</v>
       </c>
       <c r="E25" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3275,14 +3238,14 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>149</v>
+        <v>6</v>
       </c>
       <c r="B26" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
         <v>OK</v>
       </c>
       <c r="D26" t="s">
-        <v>179</v>
+        <v>157</v>
       </c>
       <c r="E26" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3291,14 +3254,14 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>150</v>
+        <v>127</v>
       </c>
       <c r="B27" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
         <v>OK</v>
       </c>
       <c r="D27" t="s">
-        <v>180</v>
+        <v>53</v>
       </c>
       <c r="E27" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3307,14 +3270,14 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>151</v>
+        <v>7</v>
       </c>
       <c r="B28" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
         <v>OK</v>
       </c>
       <c r="D28" t="s">
-        <v>181</v>
+        <v>54</v>
       </c>
       <c r="E28" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3323,14 +3286,14 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>152</v>
+        <v>8</v>
       </c>
       <c r="B29" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
         <v>OK</v>
       </c>
       <c r="D29" t="s">
-        <v>182</v>
+        <v>158</v>
       </c>
       <c r="E29" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3339,14 +3302,14 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>153</v>
+        <v>194</v>
       </c>
       <c r="B30" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
         <v>OK</v>
       </c>
       <c r="D30" t="s">
-        <v>183</v>
+        <v>55</v>
       </c>
       <c r="E30" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3355,14 +3318,14 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>154</v>
+        <v>9</v>
       </c>
       <c r="B31" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
         <v>OK</v>
       </c>
       <c r="D31" t="s">
-        <v>184</v>
+        <v>56</v>
       </c>
       <c r="E31" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3371,14 +3334,14 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="B32" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
         <v>OK</v>
       </c>
       <c r="D32" t="s">
-        <v>185</v>
+        <v>57</v>
       </c>
       <c r="E32" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3387,14 +3350,14 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="B33" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
         <v>OK</v>
       </c>
       <c r="D33" t="s">
-        <v>186</v>
+        <v>58</v>
       </c>
       <c r="E33" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3403,14 +3366,14 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>2</v>
+        <v>130</v>
       </c>
       <c r="B34" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
         <v>OK</v>
       </c>
       <c r="D34" t="s">
-        <v>187</v>
+        <v>59</v>
       </c>
       <c r="E34" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3419,14 +3382,14 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="B35" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
         <v>OK</v>
       </c>
       <c r="D35" t="s">
-        <v>188</v>
+        <v>60</v>
       </c>
       <c r="E35" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3435,14 +3398,14 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="B36" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
         <v>OK</v>
       </c>
       <c r="D36" t="s">
-        <v>189</v>
+        <v>159</v>
       </c>
       <c r="E36" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3451,14 +3414,14 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="B37" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
         <v>OK</v>
       </c>
       <c r="D37" t="s">
-        <v>190</v>
+        <v>160</v>
       </c>
       <c r="E37" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3467,14 +3430,14 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>6</v>
+        <v>131</v>
       </c>
       <c r="B38" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
         <v>OK</v>
       </c>
       <c r="D38" t="s">
-        <v>191</v>
+        <v>61</v>
       </c>
       <c r="E38" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3483,14 +3446,14 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="B39" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
         <v>OK</v>
       </c>
       <c r="D39" t="s">
-        <v>192</v>
+        <v>62</v>
       </c>
       <c r="E39" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3499,14 +3462,14 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>8</v>
+        <v>132</v>
       </c>
       <c r="B40" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
         <v>OK</v>
       </c>
       <c r="D40" t="s">
-        <v>193</v>
+        <v>161</v>
       </c>
       <c r="E40" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3515,14 +3478,14 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="B41" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
         <v>OK</v>
       </c>
       <c r="D41" t="s">
-        <v>194</v>
+        <v>162</v>
       </c>
       <c r="E41" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3531,14 +3494,14 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="B42" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
         <v>OK</v>
       </c>
       <c r="D42" t="s">
-        <v>195</v>
+        <v>163</v>
       </c>
       <c r="E42" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3547,14 +3510,14 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="B43" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
         <v>OK</v>
       </c>
       <c r="D43" t="s">
-        <v>196</v>
+        <v>63</v>
       </c>
       <c r="E43" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3563,14 +3526,14 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="B44" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
         <v>OK</v>
       </c>
       <c r="D44" t="s">
-        <v>197</v>
+        <v>64</v>
       </c>
       <c r="E44" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3579,14 +3542,14 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="B45" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
         <v>OK</v>
       </c>
       <c r="D45" t="s">
-        <v>198</v>
+        <v>65</v>
       </c>
       <c r="E45" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3595,14 +3558,14 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>13</v>
+        <v>134</v>
       </c>
       <c r="B46" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
         <v>OK</v>
       </c>
       <c r="D46" t="s">
-        <v>199</v>
+        <v>66</v>
       </c>
       <c r="E46" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3611,14 +3574,14 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>16</v>
+        <v>135</v>
       </c>
       <c r="B47" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
         <v>OK</v>
       </c>
       <c r="D47" t="s">
-        <v>41</v>
+        <v>67</v>
       </c>
       <c r="E47" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3627,14 +3590,14 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="B48" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
         <v>OK</v>
       </c>
       <c r="D48" t="s">
-        <v>42</v>
+        <v>164</v>
       </c>
       <c r="E48" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3643,14 +3606,14 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B49" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
         <v>OK</v>
       </c>
       <c r="D49" t="s">
-        <v>43</v>
+        <v>68</v>
       </c>
       <c r="E49" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3659,14 +3622,14 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>20</v>
+        <v>137</v>
       </c>
       <c r="B50" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
         <v>OK</v>
       </c>
       <c r="D50" t="s">
-        <v>44</v>
+        <v>165</v>
       </c>
       <c r="E50" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3675,14 +3638,14 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B51" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
         <v>OK</v>
       </c>
       <c r="D51" t="s">
-        <v>45</v>
+        <v>69</v>
       </c>
       <c r="E51" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3691,14 +3654,14 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B52" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
         <v>OK</v>
       </c>
       <c r="D52" t="s">
-        <v>46</v>
+        <v>166</v>
       </c>
       <c r="E52" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3707,14 +3670,14 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B53" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
         <v>OK</v>
       </c>
       <c r="D53" t="s">
-        <v>47</v>
+        <v>70</v>
       </c>
       <c r="E53" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3723,14 +3686,14 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>24</v>
+        <v>138</v>
       </c>
       <c r="B54" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
         <v>OK</v>
       </c>
       <c r="D54" t="s">
-        <v>48</v>
+        <v>71</v>
       </c>
       <c r="E54" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3739,14 +3702,14 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>25</v>
+        <v>140</v>
       </c>
       <c r="B55" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
         <v>OK</v>
       </c>
       <c r="D55" t="s">
-        <v>49</v>
+        <v>72</v>
       </c>
       <c r="E55" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3755,14 +3718,14 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B56" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
         <v>OK</v>
       </c>
       <c r="D56" t="s">
-        <v>50</v>
+        <v>167</v>
       </c>
       <c r="E56" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3771,14 +3734,14 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B57" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
         <v>OK</v>
       </c>
       <c r="D57" t="s">
-        <v>51</v>
+        <v>168</v>
       </c>
       <c r="E57" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3787,14 +3750,14 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>28</v>
+        <v>141</v>
       </c>
       <c r="B58" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
         <v>OK</v>
       </c>
       <c r="D58" t="s">
-        <v>52</v>
+        <v>169</v>
       </c>
       <c r="E58" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3803,14 +3766,14 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>29</v>
+        <v>142</v>
       </c>
       <c r="B59" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
         <v>OK</v>
       </c>
       <c r="D59" t="s">
-        <v>53</v>
+        <v>73</v>
       </c>
       <c r="E59" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3819,14 +3782,14 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B60" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
         <v>OK</v>
       </c>
       <c r="D60" t="s">
-        <v>54</v>
+        <v>74</v>
       </c>
       <c r="E60" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3835,14 +3798,14 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B61" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
         <v>OK</v>
       </c>
       <c r="D61" t="s">
-        <v>55</v>
+        <v>170</v>
       </c>
       <c r="E61" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3851,14 +3814,14 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B62" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
         <v>OK</v>
       </c>
       <c r="D62" t="s">
-        <v>56</v>
+        <v>75</v>
       </c>
       <c r="E62" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3867,14 +3830,14 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B63" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
         <v>OK</v>
       </c>
       <c r="D63" t="s">
-        <v>57</v>
+        <v>76</v>
       </c>
       <c r="E63" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3883,14 +3846,14 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B64" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
         <v>OK</v>
       </c>
       <c r="D64" t="s">
-        <v>58</v>
+        <v>77</v>
       </c>
       <c r="E64" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3899,14 +3862,14 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B65" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
         <v>OK</v>
       </c>
       <c r="D65" t="s">
-        <v>59</v>
+        <v>171</v>
       </c>
       <c r="E65" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3922,7 +3885,7 @@
         <v>OK</v>
       </c>
       <c r="D66" t="s">
-        <v>60</v>
+        <v>172</v>
       </c>
       <c r="E66" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3931,14 +3894,14 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B67" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
         <v>OK</v>
       </c>
       <c r="D67" t="s">
-        <v>61</v>
+        <v>78</v>
       </c>
       <c r="E67" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3947,14 +3910,14 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>38</v>
+        <v>143</v>
       </c>
       <c r="B68" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
         <v>OK</v>
       </c>
       <c r="D68" t="s">
-        <v>62</v>
+        <v>79</v>
       </c>
       <c r="E68" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3963,14 +3926,14 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B69" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
         <v>OK</v>
       </c>
       <c r="D69" t="s">
-        <v>63</v>
+        <v>173</v>
       </c>
       <c r="E69" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3979,59 +3942,94 @@
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
+        <v>38</v>
+      </c>
+      <c r="B70" t="str">
+        <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
+        <v>OK</v>
+      </c>
+      <c r="D70" t="s">
+        <v>80</v>
+      </c>
+      <c r="E70" t="str">
+        <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>144</v>
+      </c>
+      <c r="B71" t="str">
+        <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
+        <v>OK</v>
+      </c>
+      <c r="D71" t="s">
+        <v>81</v>
+      </c>
+      <c r="E71" t="str">
+        <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>146</v>
+      </c>
+      <c r="B72" t="str">
+        <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
+        <v>OK</v>
+      </c>
+      <c r="D72" t="s">
+        <v>82</v>
+      </c>
+      <c r="E72" t="str">
+        <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>148</v>
+      </c>
+      <c r="B73" s="16" t="str">
+        <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
+        <v>OK</v>
+      </c>
+      <c r="D73" t="s">
+        <v>83</v>
+      </c>
+      <c r="E73" t="str">
+        <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>39</v>
+      </c>
+      <c r="B74" s="16" t="str">
+        <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
+        <v>OK</v>
+      </c>
+      <c r="D74" t="s">
+        <v>84</v>
+      </c>
+      <c r="E74" t="str">
+        <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
         <v>40</v>
       </c>
-      <c r="B70" t="str">
-        <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
-        <v>OK</v>
-      </c>
-      <c r="D70" t="s">
-        <v>64</v>
-      </c>
-      <c r="E70" t="str">
-        <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
-        <v>OK</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D71" t="s">
-        <v>65</v>
-      </c>
-      <c r="E71" t="str">
-        <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
-        <v>OK</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D72" t="s">
-        <v>66</v>
-      </c>
-      <c r="E72" t="str">
-        <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
-        <v>OK</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D73" t="s">
-        <v>67</v>
-      </c>
-      <c r="E73" t="str">
-        <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
-        <v>OK</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D74" t="s">
-        <v>68</v>
-      </c>
-      <c r="E74" t="str">
-        <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
-        <v>OK</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B75" s="16" t="str">
+        <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
+        <v>OK</v>
+      </c>
       <c r="D75" t="s">
-        <v>69</v>
+        <v>85</v>
       </c>
       <c r="E75" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -4040,7 +4038,7 @@
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D76" t="s">
-        <v>70</v>
+        <v>86</v>
       </c>
       <c r="E76" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -4049,7 +4047,7 @@
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D77" t="s">
-        <v>71</v>
+        <v>87</v>
       </c>
       <c r="E77" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -4058,7 +4056,7 @@
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D78" t="s">
-        <v>72</v>
+        <v>174</v>
       </c>
       <c r="E78" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -4067,7 +4065,7 @@
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D79" t="s">
-        <v>73</v>
+        <v>88</v>
       </c>
       <c r="E79" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -4076,7 +4074,7 @@
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D80" t="s">
-        <v>74</v>
+        <v>89</v>
       </c>
       <c r="E80" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -4085,7 +4083,7 @@
     </row>
     <row r="81" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D81" t="s">
-        <v>75</v>
+        <v>175</v>
       </c>
       <c r="E81" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -4094,7 +4092,7 @@
     </row>
     <row r="82" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D82" t="s">
-        <v>76</v>
+        <v>176</v>
       </c>
       <c r="E82" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -4103,7 +4101,7 @@
     </row>
     <row r="83" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D83" t="s">
-        <v>77</v>
+        <v>177</v>
       </c>
       <c r="E83" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -4112,7 +4110,7 @@
     </row>
     <row r="84" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D84" t="s">
-        <v>78</v>
+        <v>90</v>
       </c>
       <c r="E84" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -4121,7 +4119,7 @@
     </row>
     <row r="85" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D85" t="s">
-        <v>79</v>
+        <v>91</v>
       </c>
       <c r="E85" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -4130,7 +4128,7 @@
     </row>
     <row r="86" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D86" t="s">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="E86" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -4139,7 +4137,7 @@
     </row>
     <row r="87" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D87" t="s">
-        <v>81</v>
+        <v>93</v>
       </c>
       <c r="E87" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -4148,7 +4146,7 @@
     </row>
     <row r="88" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D88" t="s">
-        <v>82</v>
+        <v>178</v>
       </c>
       <c r="E88" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -4157,7 +4155,7 @@
     </row>
     <row r="89" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D89" t="s">
-        <v>83</v>
+        <v>94</v>
       </c>
       <c r="E89" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -4166,7 +4164,7 @@
     </row>
     <row r="90" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D90" t="s">
-        <v>84</v>
+        <v>179</v>
       </c>
       <c r="E90" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -4175,7 +4173,7 @@
     </row>
     <row r="91" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D91" t="s">
-        <v>85</v>
+        <v>95</v>
       </c>
       <c r="E91" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -4184,7 +4182,7 @@
     </row>
     <row r="92" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D92" t="s">
-        <v>86</v>
+        <v>180</v>
       </c>
       <c r="E92" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -4193,7 +4191,7 @@
     </row>
     <row r="93" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D93" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="E93" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -4202,7 +4200,7 @@
     </row>
     <row r="94" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D94" t="s">
-        <v>88</v>
+        <v>97</v>
       </c>
       <c r="E94" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -4211,7 +4209,7 @@
     </row>
     <row r="95" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D95" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="E95" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -4220,7 +4218,7 @@
     </row>
     <row r="96" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D96" t="s">
-        <v>90</v>
+        <v>181</v>
       </c>
       <c r="E96" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -4229,7 +4227,7 @@
     </row>
     <row r="97" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D97" t="s">
-        <v>91</v>
+        <v>182</v>
       </c>
       <c r="E97" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -4238,7 +4236,7 @@
     </row>
     <row r="98" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D98" t="s">
-        <v>92</v>
+        <v>183</v>
       </c>
       <c r="E98" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -4247,7 +4245,7 @@
     </row>
     <row r="99" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D99" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="E99" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -4256,7 +4254,7 @@
     </row>
     <row r="100" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D100" t="s">
-        <v>94</v>
+        <v>184</v>
       </c>
       <c r="E100" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -4265,7 +4263,7 @@
     </row>
     <row r="101" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D101" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="E101" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -4274,7 +4272,7 @@
     </row>
     <row r="102" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D102" t="s">
-        <v>96</v>
+        <v>185</v>
       </c>
       <c r="E102" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -4283,7 +4281,7 @@
     </row>
     <row r="103" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D103" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="E103" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -4292,7 +4290,7 @@
     </row>
     <row r="104" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D104" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="E104" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -4301,7 +4299,7 @@
     </row>
     <row r="105" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D105" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="E105" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -4310,7 +4308,7 @@
     </row>
     <row r="106" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D106" t="s">
-        <v>100</v>
+        <v>186</v>
       </c>
       <c r="E106" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -4319,7 +4317,7 @@
     </row>
     <row r="107" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D107" t="s">
-        <v>101</v>
+        <v>187</v>
       </c>
       <c r="E107" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -4328,7 +4326,7 @@
     </row>
     <row r="108" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D108" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="E108" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -4337,7 +4335,7 @@
     </row>
     <row r="109" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D109" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="E109" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -4346,7 +4344,7 @@
     </row>
     <row r="110" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D110" t="s">
-        <v>104</v>
+        <v>188</v>
       </c>
       <c r="E110" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -4355,7 +4353,7 @@
     </row>
     <row r="111" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D111" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="E111" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -4364,7 +4362,7 @@
     </row>
     <row r="112" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D112" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="E112" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -4373,7 +4371,7 @@
     </row>
     <row r="113" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D113" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E113" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -4382,7 +4380,7 @@
     </row>
     <row r="114" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D114" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="E114" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -4391,7 +4389,7 @@
     </row>
     <row r="115" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D115" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E115" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -4400,7 +4398,7 @@
     </row>
     <row r="116" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D116" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="E116" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -4409,7 +4407,7 @@
     </row>
     <row r="117" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D117" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E117" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -4418,7 +4416,7 @@
     </row>
     <row r="118" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D118" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="E118" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -4427,7 +4425,7 @@
     </row>
     <row r="119" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D119" t="s">
-        <v>113</v>
+        <v>189</v>
       </c>
       <c r="E119" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -4454,7 +4452,7 @@
     </row>
     <row r="122" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D122" t="s">
-        <v>116</v>
+        <v>190</v>
       </c>
       <c r="E122" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -4463,7 +4461,7 @@
     </row>
     <row r="123" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D123" t="s">
-        <v>117</v>
+        <v>191</v>
       </c>
       <c r="E123" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -4472,9 +4470,36 @@
     </row>
     <row r="124" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D124" t="s">
+        <v>192</v>
+      </c>
+      <c r="E124" s="16" t="str">
+        <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="125" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D125" t="s">
+        <v>116</v>
+      </c>
+      <c r="E125" s="16" t="str">
+        <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="126" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D126" t="s">
+        <v>117</v>
+      </c>
+      <c r="E126" s="16" t="str">
+        <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="127" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D127" t="s">
         <v>118</v>
       </c>
-      <c r="E124" t="str">
+      <c r="E127" s="16" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
         <v>OK</v>
       </c>

</xml_diff>

<commit_message>
Se listo SolicitudCompra y sus Recursos en la App
</commit_message>
<xml_diff>
--- a/QuerysAñadidas.xlsx
+++ b/QuerysAñadidas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ncano\Desktop\inacons-frontend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B64D84B-1B0A-4BBD-A416-E8A628F5B4C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8999C37F-2F67-4603-96EA-9E29906FEA6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C2939682-D91A-4BD3-AD71-BB0CA9127A74}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="215">
   <si>
     <t>getAllUsuarios:[Usuario]</t>
   </si>
@@ -631,21 +631,12 @@
     <t>getCotizacionRecursoforCotizacionId(…):[CotizacionRecurso!]!</t>
   </si>
   <si>
-    <t>getCotizacionRecursoforCotizacionIdv(…):[CotizacionRecurso!]!</t>
-  </si>
-  <si>
-    <t>getCotizacionRecursov(…):CotizacionRecurso</t>
-  </si>
-  <si>
     <t>getOrdenSolicitudRecursoforSolicitudId(…):[SolicitudRecursoAlmacen!]!</t>
   </si>
   <si>
     <t>getRequerimientoAbrobacionbyRequerimientoId(…):[RequerimientoAprobacion]</t>
   </si>
   <si>
-    <t>getRequerimientoRecursoByRequerimientoIdWithAlmacenQuantities(…):[RequerimientoRecurso!]!</t>
-  </si>
-  <si>
     <t>listAlmacenCentroCostosByAlmacenId(…):[AlmacenCentroCosto!]!</t>
   </si>
   <si>
@@ -655,9 +646,6 @@
     <t>listCotizacionRecurso:[CotizacionRecurso!]!</t>
   </si>
   <si>
-    <t>listCotizacionRecursov:[CotizacionRecurso!]!</t>
-  </si>
-  <si>
     <t>listGuiaTransferenciasByTransferenciaId(…):[GuiaTransferencia!]!</t>
   </si>
   <si>
@@ -676,13 +664,22 @@
     <t>addCotizacionRecurso(…):CotizacionRecurso</t>
   </si>
   <si>
-    <t>addCotizacionRecursosv(…):CotizacionRecurso</t>
-  </si>
-  <si>
-    <t>deleteCotizacionRecursov(…):CotizacionRecurso</t>
-  </si>
-  <si>
-    <t>updateCotizacionRecursov(…):CotizacionRecurso</t>
+    <t>getRequerimientoRecursoByRequerimientoIdWithAlmacenQuantities(…):</t>
+  </si>
+  <si>
+    <t>listSolicitudCompraRecursos:[SolicitudCompraRecurso!]!</t>
+  </si>
+  <si>
+    <t>listSolicitudCompraRecursosBySolicitudId(…):[SolicitudCompraRecurso!]!</t>
+  </si>
+  <si>
+    <t>addSolicitudCompraRecurso(…):SolicitudCompraRecurso!</t>
+  </si>
+  <si>
+    <t>deleteSolicitudCompraRecurso(…):SolicitudCompraRecurso</t>
+  </si>
+  <si>
+    <t>updateSolicitudCompraRecurso(…):SolicitudCompraRecurso</t>
   </si>
 </sst>
 </file>
@@ -725,7 +722,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -786,12 +783,6 @@
         <bgColor theme="0" tint="-0.14999847407452621"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="4">
     <border>
@@ -840,7 +831,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -889,28 +880,14 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFE97132"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFE97132"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="10">
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -1084,18 +1061,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{20C6C63B-275B-4ABF-915E-BB850EBA3796}" name="Tabla1" displayName="Tabla1" ref="A1:F50" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:F50" xr:uid="{20C6C63B-275B-4ABF-915E-BB850EBA3796}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{20C6C63B-275B-4ABF-915E-BB850EBA3796}" name="Tabla1" displayName="Tabla1" ref="A1:F51" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+  <autoFilter ref="A1:F51" xr:uid="{20C6C63B-275B-4ABF-915E-BB850EBA3796}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F50">
     <sortCondition ref="B1:B50"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="2" xr3:uid="{9A32BBF7-304C-49E3-AE42-106F9CEEC961}" name="Listar" dataDxfId="9"/>
-    <tableColumn id="1" xr3:uid="{C011CDE6-69F6-4DE8-B5A1-2E6AF137E527}" name="Buscar por Id" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{7FF29903-9CE1-4BD7-849F-3471C53EC880}" name="Agregar" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{30FB0AF3-511C-4F53-947B-89013B98F552}" name="Actualizar" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{D1A0B2A0-09FE-47C4-9132-E8B248D6B643}" name="Borrar" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{C7C99C68-6028-4378-A991-EDE5C1106AD0}" name="Adicional" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{9A32BBF7-304C-49E3-AE42-106F9CEEC961}" name="Listar" dataDxfId="7"/>
+    <tableColumn id="1" xr3:uid="{C011CDE6-69F6-4DE8-B5A1-2E6AF137E527}" name="Buscar por Id" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{7FF29903-9CE1-4BD7-849F-3471C53EC880}" name="Agregar" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{30FB0AF3-511C-4F53-947B-89013B98F552}" name="Actualizar" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{D1A0B2A0-09FE-47C4-9132-E8B248D6B643}" name="Borrar" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{C7C99C68-6028-4378-A991-EDE5C1106AD0}" name="Adicional" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1109,7 +1086,7 @@
   </sortState>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{07DF1573-2247-40CE-B621-CD9F890FEE85}" name="Fields"/>
-    <tableColumn id="2" xr3:uid="{14EB541F-AFB3-43BD-B828-03CCB6D71996}" name="Esta" dataDxfId="3">
+    <tableColumn id="2" xr3:uid="{14EB541F-AFB3-43BD-B828-03CCB6D71996}" name="Esta" dataDxfId="1">
       <calculatedColumnFormula>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1120,12 +1097,12 @@
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{09B216DF-1195-4130-9747-41370EB84C29}" name="Tabla3" displayName="Tabla3" ref="D1:E127" totalsRowShown="0">
   <autoFilter ref="D1:E127" xr:uid="{09B216DF-1195-4130-9747-41370EB84C29}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="D2:E128">
-    <sortCondition ref="E1:E128"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="D2:E127">
+    <sortCondition ref="E1:E127"/>
   </sortState>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{0BA8BFE6-88AF-42D6-A824-7FA4D629D59D}" name="Fields"/>
-    <tableColumn id="2" xr3:uid="{34297603-D01A-4DD1-AEBB-FB24C3DD8C1E}" name="Esta" dataDxfId="2">
+    <tableColumn id="2" xr3:uid="{34297603-D01A-4DD1-AEBB-FB24C3DD8C1E}" name="Esta" dataDxfId="0">
       <calculatedColumnFormula>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1450,10 +1427,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DE2F4B0-FA8B-45A2-B9E1-1433688D7CE8}">
-  <dimension ref="A1:H106"/>
+  <dimension ref="A1:H104"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B50" sqref="B50"/>
+      <selection activeCell="B40" sqref="B40:B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1589,13 +1566,13 @@
     </row>
     <row r="7" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A7" s="18" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="B7" s="17" t="s">
         <v>126</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>182</v>
@@ -1667,7 +1644,7 @@
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="23"/>
       <c r="B12" s="19" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C12" s="23"/>
       <c r="D12" s="23"/>
@@ -1696,7 +1673,7 @@
         <v>29</v>
       </c>
       <c r="B14" s="18" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C14" s="7" t="s">
         <v>54</v>
@@ -1788,7 +1765,7 @@
         <v>83</v>
       </c>
       <c r="F18" s="32" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
@@ -1851,7 +1828,7 @@
         <v>130</v>
       </c>
       <c r="B22" s="18" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>149</v>
@@ -1863,7 +1840,7 @@
         <v>164</v>
       </c>
       <c r="F22" s="18" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
@@ -1927,7 +1904,7 @@
         <v>138</v>
       </c>
       <c r="B26" s="31" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>156</v>
@@ -2054,16 +2031,16 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" s="19" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="B34" s="12" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="C34" s="13"/>
       <c r="D34" s="13"/>
       <c r="E34" s="13"/>
       <c r="F34" s="12" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
@@ -2310,12 +2287,22 @@
       <c r="H50" s="14"/>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A51" s="14"/>
-      <c r="B51" s="14"/>
-      <c r="C51" s="14"/>
-      <c r="D51" s="14"/>
-      <c r="E51" s="14"/>
-      <c r="F51" s="14"/>
+      <c r="A51" s="33" t="s">
+        <v>210</v>
+      </c>
+      <c r="B51" s="33" t="s">
+        <v>211</v>
+      </c>
+      <c r="C51" s="34" t="s">
+        <v>212</v>
+      </c>
+      <c r="D51" s="34" t="s">
+        <v>214</v>
+      </c>
+      <c r="E51" s="34" t="s">
+        <v>213</v>
+      </c>
+      <c r="F51" s="13"/>
       <c r="H51" s="14"/>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.2">
@@ -2794,24 +2781,6 @@
       <c r="E104" s="14"/>
       <c r="F104" s="14"/>
       <c r="H104" s="14"/>
-    </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A105" s="14"/>
-      <c r="B105" s="14"/>
-      <c r="C105" s="14"/>
-      <c r="D105" s="14"/>
-      <c r="E105" s="14"/>
-      <c r="F105" s="14"/>
-      <c r="H105" s="14"/>
-    </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A106" s="14"/>
-      <c r="B106" s="14"/>
-      <c r="C106" s="14"/>
-      <c r="D106" s="14"/>
-      <c r="E106" s="14"/>
-      <c r="F106" s="14"/>
-      <c r="H106" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2826,7 +2795,7 @@
   <dimension ref="A1:E127"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D2:D5"/>
+      <selection activeCell="D2" sqref="D2:D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2854,7 +2823,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>196</v>
+        <v>209</v>
       </c>
       <c r="B2" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -2870,7 +2839,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>197</v>
+        <v>210</v>
       </c>
       <c r="B3" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -2881,51 +2850,51 @@
       </c>
       <c r="E3" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
-        <v>FALTA</v>
+        <v>OK</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>198</v>
+        <v>211</v>
       </c>
       <c r="B4" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
-        <v>FALTA</v>
+        <v>OK</v>
       </c>
       <c r="D4" t="s">
         <v>214</v>
       </c>
       <c r="E4" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
-        <v>FALTA</v>
+        <v>OK</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>199</v>
-      </c>
-      <c r="B5" t="str">
+        <v>207</v>
+      </c>
+      <c r="B5" s="16" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
         <v>FALTA</v>
       </c>
       <c r="D5" t="s">
-        <v>215</v>
+        <v>41</v>
       </c>
       <c r="E5" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
-        <v>FALTA</v>
+        <v>OK</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="B6" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
         <v>OK</v>
       </c>
       <c r="D6" t="s">
-        <v>41</v>
+        <v>149</v>
       </c>
       <c r="E6" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -2934,14 +2903,14 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="B7" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
         <v>OK</v>
       </c>
       <c r="D7" t="s">
-        <v>149</v>
+        <v>42</v>
       </c>
       <c r="E7" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -2950,14 +2919,14 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>202</v>
+        <v>1</v>
       </c>
       <c r="B8" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
         <v>OK</v>
       </c>
       <c r="D8" t="s">
-        <v>42</v>
+        <v>150</v>
       </c>
       <c r="E8" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -2966,14 +2935,14 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>203</v>
+        <v>2</v>
       </c>
       <c r="B9" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
         <v>OK</v>
       </c>
       <c r="D9" t="s">
-        <v>150</v>
+        <v>43</v>
       </c>
       <c r="E9" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -2982,14 +2951,14 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>204</v>
+        <v>3</v>
       </c>
       <c r="B10" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
         <v>OK</v>
       </c>
       <c r="D10" t="s">
-        <v>43</v>
+        <v>151</v>
       </c>
       <c r="E10" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -2998,14 +2967,14 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>205</v>
+        <v>4</v>
       </c>
       <c r="B11" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
         <v>OK</v>
       </c>
       <c r="D11" t="s">
-        <v>151</v>
+        <v>44</v>
       </c>
       <c r="E11" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3014,14 +2983,14 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>206</v>
+        <v>125</v>
       </c>
       <c r="B12" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
-        <v>FALTA</v>
+        <v>OK</v>
       </c>
       <c r="D12" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E12" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3030,14 +2999,14 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>207</v>
+        <v>126</v>
       </c>
       <c r="B13" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
         <v>OK</v>
       </c>
       <c r="D13" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E13" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3046,14 +3015,14 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>208</v>
+        <v>197</v>
       </c>
       <c r="B14" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
         <v>OK</v>
       </c>
       <c r="D14" t="s">
-        <v>46</v>
+        <v>152</v>
       </c>
       <c r="E14" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3062,14 +3031,14 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>209</v>
+        <v>5</v>
       </c>
       <c r="B15" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
         <v>OK</v>
       </c>
       <c r="D15" t="s">
-        <v>152</v>
+        <v>208</v>
       </c>
       <c r="E15" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3078,9 +3047,9 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>210</v>
-      </c>
-      <c r="B16" s="16" t="str">
+        <v>6</v>
+      </c>
+      <c r="B16" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
         <v>OK</v>
       </c>
@@ -3094,11 +3063,11 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>211</v>
-      </c>
-      <c r="B17" s="16" t="str">
-        <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
-        <v>FALTA</v>
+        <v>127</v>
+      </c>
+      <c r="B17" t="str">
+        <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
+        <v>OK</v>
       </c>
       <c r="D17" t="s">
         <v>47</v>
@@ -3110,7 +3079,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>0</v>
+        <v>198</v>
       </c>
       <c r="B18" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3126,7 +3095,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="B19" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3142,9 +3111,9 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>2</v>
-      </c>
-      <c r="B20" t="str">
+        <v>199</v>
+      </c>
+      <c r="B20" s="16" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
         <v>OK</v>
       </c>
@@ -3158,9 +3127,9 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>3</v>
-      </c>
-      <c r="B21" t="str">
+        <v>8</v>
+      </c>
+      <c r="B21" s="16" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
         <v>OK</v>
       </c>
@@ -3174,7 +3143,7 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>4</v>
+        <v>194</v>
       </c>
       <c r="B22" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3190,7 +3159,7 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>125</v>
+        <v>9</v>
       </c>
       <c r="B23" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3206,7 +3175,7 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>126</v>
+        <v>10</v>
       </c>
       <c r="B24" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3222,7 +3191,7 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B25" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3238,7 +3207,7 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>6</v>
+        <v>130</v>
       </c>
       <c r="B26" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3254,7 +3223,7 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>127</v>
+        <v>200</v>
       </c>
       <c r="B27" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3270,7 +3239,7 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>7</v>
+        <v>201</v>
       </c>
       <c r="B28" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3286,7 +3255,7 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B29" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3302,7 +3271,7 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>194</v>
+        <v>13</v>
       </c>
       <c r="B30" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3318,7 +3287,7 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="B31" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3334,7 +3303,7 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>10</v>
+        <v>131</v>
       </c>
       <c r="B32" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3350,7 +3319,7 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="B33" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3366,7 +3335,7 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="B34" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3382,7 +3351,7 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B35" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3398,7 +3367,7 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="B36" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3414,7 +3383,7 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="B37" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3430,7 +3399,7 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>131</v>
+        <v>20</v>
       </c>
       <c r="B38" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3446,7 +3415,7 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="B39" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3462,7 +3431,7 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>132</v>
+        <v>202</v>
       </c>
       <c r="B40" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3478,7 +3447,7 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>17</v>
+        <v>134</v>
       </c>
       <c r="B41" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3494,7 +3463,7 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>18</v>
+        <v>135</v>
       </c>
       <c r="B42" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3510,7 +3479,7 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>19</v>
+        <v>203</v>
       </c>
       <c r="B43" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3526,7 +3495,7 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B44" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3542,7 +3511,7 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B45" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3558,7 +3527,7 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="B46" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3574,7 +3543,7 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>135</v>
+        <v>24</v>
       </c>
       <c r="B47" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3590,7 +3559,7 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B48" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3606,7 +3575,7 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B49" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3622,7 +3591,7 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B50" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3638,7 +3607,7 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>24</v>
+        <v>139</v>
       </c>
       <c r="B51" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3654,7 +3623,7 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>25</v>
+        <v>140</v>
       </c>
       <c r="B52" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3670,7 +3639,7 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B53" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3686,7 +3655,7 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>138</v>
+        <v>28</v>
       </c>
       <c r="B54" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3702,7 +3671,7 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B55" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3718,7 +3687,7 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>27</v>
+        <v>142</v>
       </c>
       <c r="B56" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3734,7 +3703,7 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B57" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3750,7 +3719,7 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>141</v>
+        <v>30</v>
       </c>
       <c r="B58" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3766,7 +3735,7 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>142</v>
+        <v>31</v>
       </c>
       <c r="B59" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3782,7 +3751,7 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B60" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3798,7 +3767,7 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B61" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3814,7 +3783,7 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B62" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3830,7 +3799,7 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B63" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3846,7 +3815,7 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B64" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3862,7 +3831,7 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>34</v>
+        <v>143</v>
       </c>
       <c r="B65" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3878,7 +3847,7 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B66" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3894,7 +3863,7 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B67" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3910,7 +3879,7 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B68" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3926,7 +3895,7 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>37</v>
+        <v>205</v>
       </c>
       <c r="B69" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3942,7 +3911,7 @@
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>38</v>
+        <v>146</v>
       </c>
       <c r="B70" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3958,7 +3927,7 @@
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="B71" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3974,7 +3943,7 @@
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="B72" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3990,9 +3959,9 @@
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>148</v>
-      </c>
-      <c r="B73" s="16" t="str">
+        <v>39</v>
+      </c>
+      <c r="B73" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
         <v>OK</v>
       </c>
@@ -4006,7 +3975,7 @@
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B74" s="16" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>

</xml_diff>

<commit_message>
cotizaciones terminadas - proveedores 1%
</commit_message>
<xml_diff>
--- a/QuerysAñadidas.xlsx
+++ b/QuerysAñadidas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ncano\Desktop\inacons-frontend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8999C37F-2F67-4603-96EA-9E29906FEA6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A12B722C-D53D-40E1-8D65-12C28FDF5DF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C2939682-D91A-4BD3-AD71-BB0CA9127A74}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="225">
   <si>
     <t>getAllUsuarios:[Usuario]</t>
   </si>
@@ -43,9 +43,6 @@
     <t>getAlmacen(…):Almacen</t>
   </si>
   <si>
-    <t>getAlmacenRecurso(…):AlmacenRecurso</t>
-  </si>
-  <si>
     <t>getCompra(…):Compra</t>
   </si>
   <si>
@@ -667,19 +664,52 @@
     <t>getRequerimientoRecursoByRequerimientoIdWithAlmacenQuantities(…):</t>
   </si>
   <si>
-    <t>listSolicitudCompraRecursos:[SolicitudCompraRecurso!]!</t>
-  </si>
-  <si>
-    <t>listSolicitudCompraRecursosBySolicitudId(…):[SolicitudCompraRecurso!]!</t>
-  </si>
-  <si>
-    <t>addSolicitudCompraRecurso(…):SolicitudCompraRecurso!</t>
-  </si>
-  <si>
     <t>deleteSolicitudCompraRecurso(…):SolicitudCompraRecurso</t>
   </si>
   <si>
-    <t>updateSolicitudCompraRecurso(…):SolicitudCompraRecurso</t>
+    <t>getAlmacenRecurso(…):[AlmacenRecursoP]</t>
+  </si>
+  <si>
+    <t>getCotizacionesByProveedorId(…):[CotizacionProveedoresRecurso!]!</t>
+  </si>
+  <si>
+    <t>listCotizacionProveedores:[CotizacionProveedor!]!</t>
+  </si>
+  <si>
+    <t>listCotizacionProveedoresByCotizacionId(…):[CotizacionProveedor!]!</t>
+  </si>
+  <si>
+    <t>listCotizacionProveedoresRecursos:[CotizacionProveedoresRecurso!]!</t>
+  </si>
+  <si>
+    <t>listSolicitudCompraRecursos:[SolicitudCompraRecursoP!]!</t>
+  </si>
+  <si>
+    <t>listSolicitudCompraRecursosBySolicitudId(…):[SolicitudCompraRecursoP!]!</t>
+  </si>
+  <si>
+    <t>addCotizacionProveedor(…):CotizacionProveedor!</t>
+  </si>
+  <si>
+    <t>addCotizacionProveedoresRecurso(…):CotizacionProveedoresRecurso!</t>
+  </si>
+  <si>
+    <t>addSolicitudCompraRecurso(…):SolicitudCompraRecursoP!</t>
+  </si>
+  <si>
+    <t>deleteCotizacionProveedor(…):CotizacionProveedor</t>
+  </si>
+  <si>
+    <t>deleteCotizacionProveedoresRecurso(…):CotizacionProveedoresRecurso</t>
+  </si>
+  <si>
+    <t>updateCotizacionProveedor(…):CotizacionProveedor</t>
+  </si>
+  <si>
+    <t>updateCotizacionProveedoresRecurso(…):CotizacionProveedoresRecurso</t>
+  </si>
+  <si>
+    <t>updateSolicitudCompraRecurso(…):SolicitudCompraRecursoP</t>
   </si>
 </sst>
 </file>
@@ -722,7 +752,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -783,6 +813,18 @@
         <bgColor theme="0" tint="-0.14999847407452621"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="4">
     <border>
@@ -831,7 +873,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -877,12 +919,16 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1061,10 +1107,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{20C6C63B-275B-4ABF-915E-BB850EBA3796}" name="Tabla1" displayName="Tabla1" ref="A1:F51" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
-  <autoFilter ref="A1:F51" xr:uid="{20C6C63B-275B-4ABF-915E-BB850EBA3796}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F50">
-    <sortCondition ref="B1:B50"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{20C6C63B-275B-4ABF-915E-BB850EBA3796}" name="Tabla1" displayName="Tabla1" ref="A1:F54" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+  <autoFilter ref="A1:F54" xr:uid="{20C6C63B-275B-4ABF-915E-BB850EBA3796}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F53">
+    <sortCondition ref="B1:B53"/>
   </sortState>
   <tableColumns count="6">
     <tableColumn id="2" xr3:uid="{9A32BBF7-304C-49E3-AE42-106F9CEEC961}" name="Listar" dataDxfId="7"/>
@@ -1079,10 +1125,10 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{3DB514D5-2978-4BB5-AA4D-BEAF7ED76FD4}" name="Tabla2" displayName="Tabla2" ref="A1:B75" totalsRowShown="0">
-  <autoFilter ref="A1:B75" xr:uid="{3DB514D5-2978-4BB5-AA4D-BEAF7ED76FD4}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B75">
-    <sortCondition ref="B1:B75"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{3DB514D5-2978-4BB5-AA4D-BEAF7ED76FD4}" name="Tabla2" displayName="Tabla2" ref="A1:B78" totalsRowShown="0">
+  <autoFilter ref="A1:B78" xr:uid="{3DB514D5-2978-4BB5-AA4D-BEAF7ED76FD4}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B78">
+    <sortCondition ref="B1:B78"/>
   </sortState>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{07DF1573-2247-40CE-B621-CD9F890FEE85}" name="Fields"/>
@@ -1095,10 +1141,10 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{09B216DF-1195-4130-9747-41370EB84C29}" name="Tabla3" displayName="Tabla3" ref="D1:E127" totalsRowShown="0">
-  <autoFilter ref="D1:E127" xr:uid="{09B216DF-1195-4130-9747-41370EB84C29}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="D2:E127">
-    <sortCondition ref="E1:E127"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{09B216DF-1195-4130-9747-41370EB84C29}" name="Tabla3" displayName="Tabla3" ref="D1:E133" totalsRowShown="0">
+  <autoFilter ref="D1:E133" xr:uid="{09B216DF-1195-4130-9747-41370EB84C29}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="D2:E133">
+    <sortCondition ref="E1:E133"/>
   </sortState>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{0BA8BFE6-88AF-42D6-A824-7FA4D629D59D}" name="Fields"/>
@@ -1427,10 +1473,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DE2F4B0-FA8B-45A2-B9E1-1433688D7CE8}">
-  <dimension ref="A1:H104"/>
+  <dimension ref="A1:H99"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40:B41"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1450,886 +1496,903 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>123</v>
-      </c>
       <c r="F1" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="26" t="s">
+        <v>210</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="F3" s="4" t="s">
         <v>12</v>
-      </c>
-      <c r="B3" s="26" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F4" s="13"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>21</v>
-      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="29" t="s">
-        <v>134</v>
-      </c>
-      <c r="B6" s="29" t="s">
-        <v>125</v>
-      </c>
-      <c r="C6" s="29" t="s">
-        <v>152</v>
-      </c>
-      <c r="D6" s="29" t="s">
-        <v>181</v>
-      </c>
-      <c r="E6" s="29" t="s">
-        <v>167</v>
-      </c>
-      <c r="F6" s="13"/>
+      <c r="A6" s="37" t="s">
+        <v>133</v>
+      </c>
+      <c r="B6" s="37" t="s">
+        <v>124</v>
+      </c>
+      <c r="C6" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="D6" s="37" t="s">
+        <v>180</v>
+      </c>
+      <c r="E6" s="37" t="s">
+        <v>166</v>
+      </c>
+      <c r="F6" s="38"/>
     </row>
     <row r="7" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A7" s="18" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B7" s="17" t="s">
+        <v>125</v>
+      </c>
+      <c r="C7" s="29" t="s">
+        <v>207</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="F7" s="18" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="32" t="s">
+        <v>212</v>
+      </c>
+      <c r="B8" s="32" t="s">
+        <v>213</v>
+      </c>
+      <c r="C8" s="32" t="s">
+        <v>217</v>
+      </c>
+      <c r="D8" s="32" t="s">
+        <v>222</v>
+      </c>
+      <c r="E8" s="32" t="s">
+        <v>220</v>
+      </c>
+      <c r="F8" s="32" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="32" t="s">
+        <v>214</v>
+      </c>
+      <c r="B9" s="32"/>
+      <c r="C9" s="32" t="s">
+        <v>218</v>
+      </c>
+      <c r="D9" s="32" t="s">
+        <v>223</v>
+      </c>
+      <c r="E9" s="32" t="s">
+        <v>221</v>
+      </c>
+      <c r="F9" s="32"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="33"/>
+      <c r="B10" s="34"/>
+      <c r="C10" s="33"/>
+      <c r="D10" s="33"/>
+      <c r="E10" s="34"/>
+      <c r="F10" s="34"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="F11" s="13"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="F12" s="13"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="23"/>
+      <c r="B13" s="19" t="s">
         <v>126</v>
       </c>
-      <c r="C7" s="30" t="s">
-        <v>208</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>182</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>168</v>
-      </c>
-      <c r="F7" s="18" t="s">
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+    </row>
+    <row r="14" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="23"/>
+      <c r="B14" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="15"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="23"/>
+      <c r="B15" s="19" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="F8" s="13"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B9" s="4" t="s">
+      <c r="C15" s="23"/>
+      <c r="D15" s="23"/>
+      <c r="E15" s="23"/>
+      <c r="F15" s="23"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="F9" s="13"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="23"/>
-      <c r="B10" s="19" t="s">
-        <v>127</v>
-      </c>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-    </row>
-    <row r="11" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="23"/>
-      <c r="B11" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="C11" s="13"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="15"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" s="23"/>
-      <c r="B12" s="19" t="s">
+      <c r="C16" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" s="18" t="s">
         <v>198</v>
       </c>
-      <c r="C12" s="23"/>
-      <c r="D12" s="23"/>
-      <c r="E12" s="23"/>
-      <c r="F12" s="23"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C13" s="3" t="s">
+      <c r="C17" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D17" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="E17" s="7" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="B14" s="18" t="s">
-        <v>199</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="E14" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="F14" s="8" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="B15" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C15" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="D15" s="10" t="s">
-        <v>109</v>
-      </c>
-      <c r="E15" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="F15" s="11" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="B16" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C16" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="D16" s="10" t="s">
-        <v>109</v>
-      </c>
-      <c r="E16" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="F16" s="11" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="B17" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C17" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="D17" s="10" t="s">
-        <v>109</v>
-      </c>
-      <c r="E17" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="F17" s="11" t="s">
-        <v>184</v>
+      <c r="F17" s="8" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C18" s="28" t="s">
-        <v>56</v>
+        <v>7</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>55</v>
       </c>
       <c r="D18" s="10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="F18" s="32" t="s">
-        <v>209</v>
+        <v>82</v>
+      </c>
+      <c r="F18" s="11" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="E19" s="4" t="s">
-        <v>84</v>
+      <c r="A19" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="E19" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="F19" s="11" t="s">
+        <v>193</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B20" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="F20" s="13"/>
+      <c r="A20" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="F20" s="11" t="s">
+        <v>183</v>
+      </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="E21" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="F21" s="3" t="s">
-        <v>40</v>
+      <c r="A21" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21" s="28" t="s">
+        <v>55</v>
+      </c>
+      <c r="D21" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="E21" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="F21" s="31" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="B22" s="18" t="s">
-        <v>200</v>
+        <v>32</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>8</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>149</v>
+        <v>56</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>178</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="F22" s="18" t="s">
-        <v>201</v>
+        <v>109</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B23" s="26" t="s">
-        <v>133</v>
+        <v>35</v>
+      </c>
+      <c r="B23" s="18" t="s">
+        <v>9</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>44</v>
+        <v>58</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="E23" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="F23" s="3" t="s">
-        <v>18</v>
-      </c>
+        <v>111</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="F23" s="13"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
-        <v>135</v>
+        <v>0</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>136</v>
+        <v>10</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>153</v>
+        <v>65</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>183</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>169</v>
-      </c>
-      <c r="F24" s="13"/>
+        <v>116</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>139</v>
+        <v>129</v>
+      </c>
+      <c r="B25" s="18" t="s">
+        <v>199</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="F25" s="13"/>
-    </row>
-    <row r="26" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
+        <v>163</v>
+      </c>
+      <c r="F25" s="18" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="B26" s="31" t="s">
-        <v>204</v>
+        <v>16</v>
+      </c>
+      <c r="B26" s="26" t="s">
+        <v>132</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>156</v>
+        <v>43</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="F26" s="31" t="s">
-        <v>196</v>
+        <v>95</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="F27" s="13"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="F28" s="13"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>147</v>
+        <v>137</v>
+      </c>
+      <c r="B29" s="30" t="s">
+        <v>203</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="F29" s="13"/>
+        <v>171</v>
+      </c>
+      <c r="F29" s="30" t="s">
+        <v>195</v>
+      </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A30" s="24"/>
-      <c r="B30" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="C30" s="6"/>
-      <c r="D30" s="6"/>
-      <c r="E30" s="6"/>
-      <c r="F30" s="6"/>
+      <c r="A30" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="F30" s="13"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="B31" s="13"/>
+        <v>143</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>144</v>
+      </c>
       <c r="C31" s="3" t="s">
-        <v>150</v>
+        <v>161</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>179</v>
+        <v>190</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>165</v>
+        <v>175</v>
       </c>
       <c r="F31" s="13"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
-        <v>16</v>
+        <v>145</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>146</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>43</v>
+        <v>162</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="E32" s="4" t="s">
-        <v>69</v>
-      </c>
+        <v>191</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="F32" s="13"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A33" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="B33" s="13"/>
-      <c r="C33" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>180</v>
-      </c>
-      <c r="E33" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="F33" s="20"/>
+      <c r="A33" s="24"/>
+      <c r="B33" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="C33" s="6"/>
+      <c r="D33" s="6"/>
+      <c r="E33" s="6"/>
+      <c r="F33" s="6"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A34" s="19" t="s">
-        <v>203</v>
-      </c>
-      <c r="B34" s="12" t="s">
-        <v>205</v>
-      </c>
-      <c r="C34" s="13"/>
-      <c r="D34" s="13"/>
-      <c r="E34" s="13"/>
-      <c r="F34" s="12" t="s">
-        <v>206</v>
-      </c>
+      <c r="A34" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="B34" s="13"/>
+      <c r="C34" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="F34" s="13"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A35" s="4" t="s">
-        <v>22</v>
+      <c r="A35" s="3" t="s">
+        <v>15</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="D35" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="E35" s="3" t="s">
-        <v>73</v>
+        <v>42</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="B36" s="13"/>
       <c r="C36" s="3" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="F36" s="13"/>
+        <v>165</v>
+      </c>
+      <c r="F36" s="20"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A37" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B37" s="13"/>
-      <c r="C37" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="D37" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="E37" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="F37" s="13"/>
+      <c r="A37" s="19" t="s">
+        <v>202</v>
+      </c>
+      <c r="B37" s="12" t="s">
+        <v>204</v>
+      </c>
+      <c r="C37" s="13"/>
+      <c r="D37" s="13"/>
+      <c r="E37" s="13"/>
+      <c r="F37" s="12" t="s">
+        <v>205</v>
+      </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A38" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B38" s="13"/>
+      <c r="A38" s="4" t="s">
+        <v>21</v>
+      </c>
       <c r="C38" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="D38" s="3" t="s">
-        <v>102</v>
+        <v>117</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>98</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="F38" s="13"/>
+        <v>72</v>
+      </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
-        <v>27</v>
-      </c>
+        <v>136</v>
+      </c>
+      <c r="B39" s="13"/>
       <c r="C39" s="3" t="s">
-        <v>51</v>
+        <v>153</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="E39" s="4" t="s">
-        <v>78</v>
-      </c>
+        <v>184</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="F39" s="13"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
-        <v>28</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="B40" s="13"/>
       <c r="C40" s="3" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="E40" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="F40" s="3" t="s">
-        <v>65</v>
-      </c>
+        <v>102</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="F40" s="13"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B41" s="13"/>
       <c r="C41" s="3" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="F41" s="13"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B42" s="13"/>
+        <v>26</v>
+      </c>
       <c r="C42" s="3" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="E42" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="F42" s="22"/>
+        <v>103</v>
+      </c>
+      <c r="E42" s="4" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B43" s="13"/>
+        <v>27</v>
+      </c>
       <c r="C43" s="3" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="E43" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="F43" s="22"/>
+        <v>104</v>
+      </c>
+      <c r="E43" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="F43" s="3" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A44" s="17" t="s">
-        <v>143</v>
+      <c r="A44" s="3" t="s">
+        <v>29</v>
       </c>
       <c r="B44" s="13"/>
       <c r="C44" s="3" t="s">
-        <v>160</v>
+        <v>54</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>189</v>
+        <v>107</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>174</v>
+        <v>81</v>
       </c>
       <c r="F44" s="13"/>
-      <c r="H44" s="14"/>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A45" s="17" t="s">
-        <v>37</v>
-      </c>
+      <c r="A45" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B45" s="13"/>
       <c r="C45" s="3" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="E45" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="H45" s="14"/>
+        <v>110</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="F45" s="22"/>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A46" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="B46" s="25"/>
+      <c r="A46" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B46" s="13"/>
       <c r="C46" s="3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="E46" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="H46" s="14"/>
+        <v>112</v>
+      </c>
+      <c r="E46" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="F46" s="22"/>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" s="17" t="s">
-        <v>148</v>
-      </c>
+        <v>142</v>
+      </c>
+      <c r="B47" s="13"/>
       <c r="C47" s="3" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="F47" s="23"/>
+        <v>173</v>
+      </c>
+      <c r="F47" s="13"/>
       <c r="H47" s="14"/>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A48" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="B48" s="25"/>
+      <c r="A48" s="17" t="s">
+        <v>36</v>
+      </c>
       <c r="C48" s="3" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="E48" s="4" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="H48" s="14"/>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A49" s="23"/>
-      <c r="B49" s="20"/>
-      <c r="C49" s="13"/>
-      <c r="D49" s="13"/>
-      <c r="E49" s="13"/>
-      <c r="F49" s="21" t="s">
+      <c r="A49" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="B49" s="25"/>
+      <c r="C49" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="E49" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="H49" s="14"/>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A50" s="17" t="s">
+        <v>147</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="E50" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="F50" s="23"/>
+      <c r="H50" s="14"/>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A51" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="B51" s="25"/>
+      <c r="C51" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="E51" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="H51" s="14"/>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A52" s="23"/>
+      <c r="B52" s="20"/>
+      <c r="C52" s="13"/>
+      <c r="D52" s="13"/>
+      <c r="E52" s="13"/>
+      <c r="F52" s="21" t="s">
+        <v>157</v>
+      </c>
+      <c r="H52" s="14"/>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A53" s="23"/>
+      <c r="B53" s="27"/>
+      <c r="C53" s="13"/>
+      <c r="D53" s="13"/>
+      <c r="E53" s="13"/>
+      <c r="F53" s="21" t="s">
         <v>158</v>
       </c>
-      <c r="H49" s="14"/>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A50" s="23"/>
-      <c r="B50" s="27"/>
-      <c r="C50" s="13"/>
-      <c r="D50" s="13"/>
-      <c r="E50" s="13"/>
-      <c r="F50" s="21" t="s">
-        <v>159</v>
-      </c>
-      <c r="H50" s="14"/>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A51" s="33" t="s">
-        <v>210</v>
-      </c>
-      <c r="B51" s="33" t="s">
-        <v>211</v>
-      </c>
-      <c r="C51" s="34" t="s">
-        <v>212</v>
-      </c>
-      <c r="D51" s="34" t="s">
-        <v>214</v>
-      </c>
-      <c r="E51" s="34" t="s">
-        <v>213</v>
-      </c>
-      <c r="F51" s="13"/>
-      <c r="H51" s="14"/>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A52" s="14"/>
-      <c r="B52" s="14"/>
-      <c r="C52" s="14"/>
-      <c r="D52" s="14"/>
-      <c r="E52" s="14"/>
-      <c r="F52" s="14"/>
-      <c r="H52" s="14"/>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A53" s="14"/>
-      <c r="B53" s="14"/>
-      <c r="C53" s="14"/>
-      <c r="D53" s="14"/>
-      <c r="E53" s="14"/>
-      <c r="F53" s="14"/>
       <c r="H53" s="14"/>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A54" s="14"/>
-      <c r="B54" s="14"/>
-      <c r="C54" s="14"/>
-      <c r="D54" s="14"/>
-      <c r="E54" s="14"/>
-      <c r="F54" s="14"/>
+      <c r="A54" s="35" t="s">
+        <v>215</v>
+      </c>
+      <c r="B54" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="C54" s="36" t="s">
+        <v>219</v>
+      </c>
+      <c r="D54" s="36" t="s">
+        <v>224</v>
+      </c>
+      <c r="E54" s="36" t="s">
+        <v>209</v>
+      </c>
+      <c r="F54" s="13"/>
       <c r="H54" s="14"/>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.2">
@@ -2736,51 +2799,6 @@
       <c r="E99" s="14"/>
       <c r="F99" s="14"/>
       <c r="H99" s="14"/>
-    </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A100" s="14"/>
-      <c r="B100" s="14"/>
-      <c r="C100" s="14"/>
-      <c r="D100" s="14"/>
-      <c r="E100" s="14"/>
-      <c r="F100" s="14"/>
-      <c r="H100" s="14"/>
-    </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A101" s="14"/>
-      <c r="B101" s="14"/>
-      <c r="C101" s="14"/>
-      <c r="D101" s="14"/>
-      <c r="E101" s="14"/>
-      <c r="F101" s="14"/>
-      <c r="H101" s="14"/>
-    </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A102" s="14"/>
-      <c r="B102" s="14"/>
-      <c r="C102" s="14"/>
-      <c r="D102" s="14"/>
-      <c r="E102" s="14"/>
-      <c r="F102" s="14"/>
-      <c r="H102" s="14"/>
-    </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A103" s="14"/>
-      <c r="B103" s="14"/>
-      <c r="C103" s="14"/>
-      <c r="D103" s="14"/>
-      <c r="E103" s="14"/>
-      <c r="F103" s="14"/>
-      <c r="H103" s="14"/>
-    </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A104" s="14"/>
-      <c r="B104" s="14"/>
-      <c r="C104" s="14"/>
-      <c r="D104" s="14"/>
-      <c r="E104" s="14"/>
-      <c r="F104" s="14"/>
-      <c r="H104" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2792,10 +2810,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E7E83A2-0C01-4873-A759-2E5A62E8D39F}">
-  <dimension ref="A1:E127"/>
+  <dimension ref="A1:E133"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D4"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2809,28 +2827,28 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>209</v>
-      </c>
-      <c r="B2" t="str">
+        <v>210</v>
+      </c>
+      <c r="B2" s="16" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
         <v>OK</v>
       </c>
       <c r="D2" t="s">
-        <v>212</v>
+        <v>217</v>
       </c>
       <c r="E2" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -2839,14 +2857,14 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B3" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
         <v>OK</v>
       </c>
       <c r="D3" t="s">
-        <v>213</v>
+        <v>218</v>
       </c>
       <c r="E3" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -2855,14 +2873,14 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B4" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
         <v>OK</v>
       </c>
       <c r="D4" t="s">
-        <v>214</v>
+        <v>219</v>
       </c>
       <c r="E4" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -2871,14 +2889,14 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>207</v>
-      </c>
-      <c r="B5" s="16" t="str">
-        <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
-        <v>FALTA</v>
+        <v>213</v>
+      </c>
+      <c r="B5" t="str">
+        <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
+        <v>OK</v>
       </c>
       <c r="D5" t="s">
-        <v>41</v>
+        <v>220</v>
       </c>
       <c r="E5" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -2887,14 +2905,14 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>196</v>
+        <v>214</v>
       </c>
       <c r="B6" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
         <v>OK</v>
       </c>
       <c r="D6" t="s">
-        <v>149</v>
+        <v>221</v>
       </c>
       <c r="E6" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -2903,14 +2921,14 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>0</v>
+        <v>215</v>
       </c>
       <c r="B7" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
         <v>OK</v>
       </c>
       <c r="D7" t="s">
-        <v>42</v>
+        <v>222</v>
       </c>
       <c r="E7" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -2919,14 +2937,14 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>1</v>
+        <v>216</v>
       </c>
       <c r="B8" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
         <v>OK</v>
       </c>
       <c r="D8" t="s">
-        <v>150</v>
+        <v>223</v>
       </c>
       <c r="E8" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -2935,14 +2953,14 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>2</v>
-      </c>
-      <c r="B9" t="str">
-        <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
-        <v>OK</v>
+        <v>206</v>
+      </c>
+      <c r="B9" s="16" t="str">
+        <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
+        <v>FALTA</v>
       </c>
       <c r="D9" t="s">
-        <v>43</v>
+        <v>224</v>
       </c>
       <c r="E9" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -2951,14 +2969,14 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>3</v>
+        <v>195</v>
       </c>
       <c r="B10" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
         <v>OK</v>
       </c>
       <c r="D10" t="s">
-        <v>151</v>
+        <v>40</v>
       </c>
       <c r="E10" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -2967,14 +2985,14 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B11" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
         <v>OK</v>
       </c>
       <c r="D11" t="s">
-        <v>44</v>
+        <v>148</v>
       </c>
       <c r="E11" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -2983,14 +3001,14 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>125</v>
+        <v>1</v>
       </c>
       <c r="B12" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
         <v>OK</v>
       </c>
       <c r="D12" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="E12" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -2999,14 +3017,14 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>126</v>
+        <v>2</v>
       </c>
       <c r="B13" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
         <v>OK</v>
       </c>
       <c r="D13" t="s">
-        <v>46</v>
+        <v>149</v>
       </c>
       <c r="E13" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3015,14 +3033,14 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>197</v>
+        <v>3</v>
       </c>
       <c r="B14" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
         <v>OK</v>
       </c>
       <c r="D14" t="s">
-        <v>152</v>
+        <v>42</v>
       </c>
       <c r="E14" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3031,14 +3049,14 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>5</v>
+        <v>124</v>
       </c>
       <c r="B15" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
         <v>OK</v>
       </c>
       <c r="D15" t="s">
-        <v>208</v>
+        <v>150</v>
       </c>
       <c r="E15" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3047,14 +3065,14 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>6</v>
+        <v>125</v>
       </c>
       <c r="B16" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
         <v>OK</v>
       </c>
       <c r="D16" t="s">
-        <v>153</v>
+        <v>43</v>
       </c>
       <c r="E16" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3063,14 +3081,14 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>127</v>
+        <v>196</v>
       </c>
       <c r="B17" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
         <v>OK</v>
       </c>
       <c r="D17" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E17" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3079,14 +3097,14 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>198</v>
+        <v>4</v>
       </c>
       <c r="B18" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
         <v>OK</v>
       </c>
       <c r="D18" t="s">
-        <v>154</v>
+        <v>45</v>
       </c>
       <c r="E18" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3095,14 +3113,14 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B19" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
         <v>OK</v>
       </c>
       <c r="D19" t="s">
-        <v>48</v>
+        <v>151</v>
       </c>
       <c r="E19" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3111,14 +3129,14 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>199</v>
-      </c>
-      <c r="B20" s="16" t="str">
+        <v>126</v>
+      </c>
+      <c r="B20" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
         <v>OK</v>
       </c>
       <c r="D20" t="s">
-        <v>49</v>
+        <v>207</v>
       </c>
       <c r="E20" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3127,14 +3145,14 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>8</v>
-      </c>
-      <c r="B21" s="16" t="str">
+        <v>197</v>
+      </c>
+      <c r="B21" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
         <v>OK</v>
       </c>
       <c r="D21" t="s">
-        <v>50</v>
+        <v>152</v>
       </c>
       <c r="E21" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3143,14 +3161,14 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>194</v>
+        <v>6</v>
       </c>
       <c r="B22" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
         <v>OK</v>
       </c>
       <c r="D22" t="s">
-        <v>155</v>
+        <v>46</v>
       </c>
       <c r="E22" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3159,14 +3177,14 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>9</v>
+        <v>198</v>
       </c>
       <c r="B23" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
         <v>OK</v>
       </c>
       <c r="D23" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="E23" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3175,14 +3193,14 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B24" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
         <v>OK</v>
       </c>
       <c r="D24" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E24" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3191,14 +3209,14 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>11</v>
+        <v>193</v>
       </c>
       <c r="B25" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
         <v>OK</v>
       </c>
       <c r="D25" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="E25" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3207,14 +3225,14 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>130</v>
-      </c>
-      <c r="B26" t="str">
+        <v>208</v>
+      </c>
+      <c r="B26" s="16" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
         <v>OK</v>
       </c>
       <c r="D26" t="s">
-        <v>157</v>
+        <v>49</v>
       </c>
       <c r="E26" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3223,14 +3241,14 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>200</v>
-      </c>
-      <c r="B27" t="str">
+        <v>8</v>
+      </c>
+      <c r="B27" s="16" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
         <v>OK</v>
       </c>
       <c r="D27" t="s">
-        <v>53</v>
+        <v>154</v>
       </c>
       <c r="E27" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3239,14 +3257,14 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>201</v>
+        <v>9</v>
       </c>
       <c r="B28" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
         <v>OK</v>
       </c>
       <c r="D28" t="s">
-        <v>54</v>
+        <v>155</v>
       </c>
       <c r="E28" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3255,14 +3273,14 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B29" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
         <v>OK</v>
       </c>
       <c r="D29" t="s">
-        <v>158</v>
+        <v>50</v>
       </c>
       <c r="E29" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3271,14 +3289,14 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>13</v>
+        <v>129</v>
       </c>
       <c r="B30" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
         <v>OK</v>
       </c>
       <c r="D30" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="E30" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3287,14 +3305,14 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>14</v>
+        <v>199</v>
       </c>
       <c r="B31" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
         <v>OK</v>
       </c>
       <c r="D31" t="s">
-        <v>56</v>
+        <v>156</v>
       </c>
       <c r="E31" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3303,14 +3321,14 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>131</v>
+        <v>200</v>
       </c>
       <c r="B32" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
         <v>OK</v>
       </c>
       <c r="D32" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="E32" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3319,14 +3337,14 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B33" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
         <v>OK</v>
       </c>
       <c r="D33" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="E33" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3335,14 +3353,14 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>132</v>
+        <v>12</v>
       </c>
       <c r="B34" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
         <v>OK</v>
       </c>
       <c r="D34" t="s">
-        <v>59</v>
+        <v>157</v>
       </c>
       <c r="E34" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3351,14 +3369,14 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B35" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
         <v>OK</v>
       </c>
       <c r="D35" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="E35" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3367,14 +3385,14 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>18</v>
+        <v>130</v>
       </c>
       <c r="B36" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
         <v>OK</v>
       </c>
       <c r="D36" t="s">
-        <v>159</v>
+        <v>55</v>
       </c>
       <c r="E36" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3383,14 +3401,14 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B37" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
         <v>OK</v>
       </c>
       <c r="D37" t="s">
-        <v>160</v>
+        <v>56</v>
       </c>
       <c r="E37" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3399,14 +3417,14 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>20</v>
+        <v>131</v>
       </c>
       <c r="B38" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
         <v>OK</v>
       </c>
       <c r="D38" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E38" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3415,14 +3433,14 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B39" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
         <v>OK</v>
       </c>
       <c r="D39" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E39" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3431,14 +3449,14 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>202</v>
+        <v>17</v>
       </c>
       <c r="B40" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
         <v>OK</v>
       </c>
       <c r="D40" t="s">
-        <v>161</v>
+        <v>59</v>
       </c>
       <c r="E40" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3447,14 +3465,14 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>134</v>
+        <v>18</v>
       </c>
       <c r="B41" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
         <v>OK</v>
       </c>
       <c r="D41" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="E41" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3463,14 +3481,14 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>135</v>
+        <v>19</v>
       </c>
       <c r="B42" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
         <v>OK</v>
       </c>
       <c r="D42" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="E42" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3479,14 +3497,14 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>203</v>
+        <v>20</v>
       </c>
       <c r="B43" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
         <v>OK</v>
       </c>
       <c r="D43" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E43" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3495,14 +3513,14 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>22</v>
+        <v>201</v>
       </c>
       <c r="B44" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
         <v>OK</v>
       </c>
       <c r="D44" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E44" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3511,14 +3529,14 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>23</v>
+        <v>133</v>
       </c>
       <c r="B45" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
         <v>OK</v>
       </c>
       <c r="D45" t="s">
-        <v>65</v>
+        <v>160</v>
       </c>
       <c r="E45" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3527,14 +3545,14 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B46" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
         <v>OK</v>
       </c>
       <c r="D46" t="s">
-        <v>66</v>
+        <v>161</v>
       </c>
       <c r="E46" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3543,14 +3561,14 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>24</v>
+        <v>202</v>
       </c>
       <c r="B47" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
         <v>OK</v>
       </c>
       <c r="D47" t="s">
-        <v>67</v>
+        <v>162</v>
       </c>
       <c r="E47" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3559,14 +3577,14 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B48" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
         <v>OK</v>
       </c>
       <c r="D48" t="s">
-        <v>164</v>
+        <v>62</v>
       </c>
       <c r="E48" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3575,14 +3593,14 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B49" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
         <v>OK</v>
       </c>
       <c r="D49" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="E49" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3591,14 +3609,14 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B50" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
         <v>OK</v>
       </c>
       <c r="D50" t="s">
-        <v>165</v>
+        <v>64</v>
       </c>
       <c r="E50" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3607,14 +3625,14 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>139</v>
+        <v>23</v>
       </c>
       <c r="B51" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
         <v>OK</v>
       </c>
       <c r="D51" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="E51" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3623,14 +3641,14 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>140</v>
+        <v>24</v>
       </c>
       <c r="B52" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
         <v>OK</v>
       </c>
       <c r="D52" t="s">
-        <v>166</v>
+        <v>66</v>
       </c>
       <c r="E52" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3639,14 +3657,14 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B53" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
         <v>OK</v>
       </c>
       <c r="D53" t="s">
-        <v>70</v>
+        <v>163</v>
       </c>
       <c r="E53" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3655,14 +3673,14 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>28</v>
+        <v>137</v>
       </c>
       <c r="B54" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
         <v>OK</v>
       </c>
       <c r="D54" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="E54" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3671,14 +3689,14 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B55" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
         <v>OK</v>
       </c>
       <c r="D55" t="s">
-        <v>72</v>
+        <v>164</v>
       </c>
       <c r="E55" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3687,14 +3705,14 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B56" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
         <v>OK</v>
       </c>
       <c r="D56" t="s">
-        <v>167</v>
+        <v>68</v>
       </c>
       <c r="E56" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3703,14 +3721,14 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B57" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
         <v>OK</v>
       </c>
       <c r="D57" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="E57" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3719,14 +3737,14 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B58" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
         <v>OK</v>
       </c>
       <c r="D58" t="s">
-        <v>169</v>
+        <v>69</v>
       </c>
       <c r="E58" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3735,14 +3753,14 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>31</v>
+        <v>140</v>
       </c>
       <c r="B59" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
         <v>OK</v>
       </c>
       <c r="D59" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E59" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3751,14 +3769,14 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>32</v>
+        <v>141</v>
       </c>
       <c r="B60" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
         <v>OK</v>
       </c>
       <c r="D60" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E60" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3767,14 +3785,14 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B61" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
         <v>OK</v>
       </c>
       <c r="D61" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="E61" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3783,14 +3801,14 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B62" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
         <v>OK</v>
       </c>
       <c r="D62" t="s">
-        <v>75</v>
+        <v>167</v>
       </c>
       <c r="E62" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3799,14 +3817,14 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B63" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
         <v>OK</v>
       </c>
       <c r="D63" t="s">
-        <v>76</v>
+        <v>168</v>
       </c>
       <c r="E63" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3815,14 +3833,14 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B64" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
         <v>OK</v>
       </c>
       <c r="D64" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="E64" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3831,14 +3849,14 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>143</v>
+        <v>32</v>
       </c>
       <c r="B65" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
         <v>OK</v>
       </c>
       <c r="D65" t="s">
-        <v>171</v>
+        <v>73</v>
       </c>
       <c r="E65" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3847,14 +3865,14 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B66" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
         <v>OK</v>
       </c>
       <c r="D66" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="E66" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3863,14 +3881,14 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B67" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
         <v>OK</v>
       </c>
       <c r="D67" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="E67" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3879,14 +3897,14 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>144</v>
+        <v>35</v>
       </c>
       <c r="B68" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
         <v>OK</v>
       </c>
       <c r="D68" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="E68" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3895,14 +3913,14 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>205</v>
+        <v>142</v>
       </c>
       <c r="B69" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
         <v>OK</v>
       </c>
       <c r="D69" t="s">
-        <v>173</v>
+        <v>76</v>
       </c>
       <c r="E69" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3911,14 +3929,14 @@
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>146</v>
+        <v>36</v>
       </c>
       <c r="B70" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
         <v>OK</v>
       </c>
       <c r="D70" t="s">
-        <v>80</v>
+        <v>170</v>
       </c>
       <c r="E70" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3927,14 +3945,14 @@
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>147</v>
+        <v>37</v>
       </c>
       <c r="B71" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
         <v>OK</v>
       </c>
       <c r="D71" t="s">
-        <v>81</v>
+        <v>171</v>
       </c>
       <c r="E71" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3943,14 +3961,14 @@
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="B72" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
         <v>OK</v>
       </c>
       <c r="D72" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="E72" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3959,14 +3977,14 @@
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>39</v>
+        <v>204</v>
       </c>
       <c r="B73" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
         <v>OK</v>
       </c>
       <c r="D73" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="E73" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3975,14 +3993,14 @@
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>40</v>
-      </c>
-      <c r="B74" s="16" t="str">
+        <v>145</v>
+      </c>
+      <c r="B74" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
         <v>OK</v>
       </c>
       <c r="D74" t="s">
-        <v>84</v>
+        <v>172</v>
       </c>
       <c r="E74" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -3991,14 +4009,14 @@
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>40</v>
+        <v>146</v>
       </c>
       <c r="B75" s="16" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
         <v>OK</v>
       </c>
       <c r="D75" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="E75" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -4006,8 +4024,15 @@
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>147</v>
+      </c>
+      <c r="B76" s="16" t="str">
+        <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
+        <v>OK</v>
+      </c>
       <c r="D76" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="E76" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -4015,8 +4040,15 @@
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>38</v>
+      </c>
+      <c r="B77" s="16" t="str">
+        <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
+        <v>OK</v>
+      </c>
       <c r="D77" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="E77" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -4024,8 +4056,15 @@
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>39</v>
+      </c>
+      <c r="B78" s="16" t="str">
+        <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla2[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
+        <v>OK</v>
+      </c>
       <c r="D78" t="s">
-        <v>174</v>
+        <v>82</v>
       </c>
       <c r="E78" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -4034,7 +4073,7 @@
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D79" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="E79" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -4043,7 +4082,7 @@
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D80" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="E80" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -4052,7 +4091,7 @@
     </row>
     <row r="81" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D81" t="s">
-        <v>175</v>
+        <v>85</v>
       </c>
       <c r="E81" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -4061,7 +4100,7 @@
     </row>
     <row r="82" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D82" t="s">
-        <v>176</v>
+        <v>209</v>
       </c>
       <c r="E82" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -4070,7 +4109,7 @@
     </row>
     <row r="83" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D83" t="s">
-        <v>177</v>
+        <v>86</v>
       </c>
       <c r="E83" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -4079,7 +4118,7 @@
     </row>
     <row r="84" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D84" t="s">
-        <v>90</v>
+        <v>173</v>
       </c>
       <c r="E84" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -4088,7 +4127,7 @@
     </row>
     <row r="85" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D85" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="E85" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -4097,7 +4136,7 @@
     </row>
     <row r="86" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D86" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="E86" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -4106,7 +4145,7 @@
     </row>
     <row r="87" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D87" t="s">
-        <v>93</v>
+        <v>174</v>
       </c>
       <c r="E87" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -4115,7 +4154,7 @@
     </row>
     <row r="88" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D88" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="E88" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -4124,7 +4163,7 @@
     </row>
     <row r="89" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D89" t="s">
-        <v>94</v>
+        <v>176</v>
       </c>
       <c r="E89" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -4133,7 +4172,7 @@
     </row>
     <row r="90" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D90" t="s">
-        <v>179</v>
+        <v>89</v>
       </c>
       <c r="E90" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -4142,7 +4181,7 @@
     </row>
     <row r="91" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D91" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="E91" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -4151,7 +4190,7 @@
     </row>
     <row r="92" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D92" t="s">
-        <v>180</v>
+        <v>91</v>
       </c>
       <c r="E92" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -4160,7 +4199,7 @@
     </row>
     <row r="93" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D93" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="E93" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -4169,7 +4208,7 @@
     </row>
     <row r="94" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D94" t="s">
-        <v>97</v>
+        <v>177</v>
       </c>
       <c r="E94" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -4178,7 +4217,7 @@
     </row>
     <row r="95" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D95" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="E95" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -4187,7 +4226,7 @@
     </row>
     <row r="96" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D96" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="E96" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -4196,7 +4235,7 @@
     </row>
     <row r="97" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D97" t="s">
-        <v>182</v>
+        <v>94</v>
       </c>
       <c r="E97" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -4205,7 +4244,7 @@
     </row>
     <row r="98" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D98" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="E98" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -4214,7 +4253,7 @@
     </row>
     <row r="99" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D99" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="E99" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -4223,7 +4262,7 @@
     </row>
     <row r="100" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D100" t="s">
-        <v>184</v>
+        <v>96</v>
       </c>
       <c r="E100" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -4232,7 +4271,7 @@
     </row>
     <row r="101" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D101" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="E101" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -4241,7 +4280,7 @@
     </row>
     <row r="102" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D102" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="E102" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -4250,7 +4289,7 @@
     </row>
     <row r="103" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D103" t="s">
-        <v>101</v>
+        <v>181</v>
       </c>
       <c r="E103" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -4259,7 +4298,7 @@
     </row>
     <row r="104" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D104" t="s">
-        <v>102</v>
+        <v>182</v>
       </c>
       <c r="E104" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -4268,7 +4307,7 @@
     </row>
     <row r="105" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D105" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="E105" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -4277,7 +4316,7 @@
     </row>
     <row r="106" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D106" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="E106" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -4286,7 +4325,7 @@
     </row>
     <row r="107" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D107" t="s">
-        <v>187</v>
+        <v>99</v>
       </c>
       <c r="E107" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -4295,7 +4334,7 @@
     </row>
     <row r="108" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D108" t="s">
-        <v>104</v>
+        <v>184</v>
       </c>
       <c r="E108" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -4304,7 +4343,7 @@
     </row>
     <row r="109" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D109" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="E109" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -4313,7 +4352,7 @@
     </row>
     <row r="110" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D110" t="s">
-        <v>188</v>
+        <v>101</v>
       </c>
       <c r="E110" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -4322,7 +4361,7 @@
     </row>
     <row r="111" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D111" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="E111" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -4331,7 +4370,7 @@
     </row>
     <row r="112" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D112" t="s">
-        <v>107</v>
+        <v>185</v>
       </c>
       <c r="E112" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -4340,7 +4379,7 @@
     </row>
     <row r="113" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D113" t="s">
-        <v>108</v>
+        <v>186</v>
       </c>
       <c r="E113" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -4349,7 +4388,7 @@
     </row>
     <row r="114" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D114" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="E114" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -4358,7 +4397,7 @@
     </row>
     <row r="115" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D115" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="E115" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -4367,7 +4406,7 @@
     </row>
     <row r="116" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D116" t="s">
-        <v>111</v>
+        <v>187</v>
       </c>
       <c r="E116" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -4376,7 +4415,7 @@
     </row>
     <row r="117" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D117" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="E117" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -4385,7 +4424,7 @@
     </row>
     <row r="118" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D118" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="E118" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -4394,7 +4433,7 @@
     </row>
     <row r="119" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D119" t="s">
-        <v>189</v>
+        <v>107</v>
       </c>
       <c r="E119" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -4403,7 +4442,7 @@
     </row>
     <row r="120" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D120" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="E120" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -4412,7 +4451,7 @@
     </row>
     <row r="121" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D121" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="E121" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -4421,7 +4460,7 @@
     </row>
     <row r="122" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D122" t="s">
-        <v>190</v>
+        <v>110</v>
       </c>
       <c r="E122" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -4430,7 +4469,7 @@
     </row>
     <row r="123" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D123" t="s">
-        <v>191</v>
+        <v>111</v>
       </c>
       <c r="E123" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -4439,7 +4478,7 @@
     </row>
     <row r="124" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D124" t="s">
-        <v>192</v>
+        <v>112</v>
       </c>
       <c r="E124" s="16" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -4448,7 +4487,7 @@
     </row>
     <row r="125" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D125" t="s">
-        <v>116</v>
+        <v>188</v>
       </c>
       <c r="E125" s="16" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -4457,7 +4496,7 @@
     </row>
     <row r="126" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D126" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="E126" s="16" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
@@ -4466,9 +4505,63 @@
     </row>
     <row r="127" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D127" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="E127" s="16" t="str">
+        <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="128" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D128" t="s">
+        <v>189</v>
+      </c>
+      <c r="E128" s="16" t="str">
+        <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="129" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D129" t="s">
+        <v>190</v>
+      </c>
+      <c r="E129" s="16" t="str">
+        <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="130" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D130" t="s">
+        <v>191</v>
+      </c>
+      <c r="E130" s="16" t="str">
+        <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="131" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D131" t="s">
+        <v>115</v>
+      </c>
+      <c r="E131" s="16" t="str">
+        <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="132" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D132" t="s">
+        <v>116</v>
+      </c>
+      <c r="E132" s="16" t="str">
+        <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
+        <v>OK</v>
+      </c>
+    </row>
+    <row r="133" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D133" t="s">
+        <v>117</v>
+      </c>
+      <c r="E133" s="16" t="str">
         <f>IF(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(IFERROR(VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Listar],1,0),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Buscar por Id],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Agregar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Actualizar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Borrar],1,0)),VLOOKUP(Tabla3[[#This Row],[Fields]],Tabla1[Adicional],1,0)),"FALTA")="FALTA","FALTA","OK")</f>
         <v>OK</v>
       </c>

</xml_diff>